<commit_message>
problem 347 both using heapq data structures and counter method most_common
</commit_message>
<xml_diff>
--- a/Leetcode Team 403 Habiter.xlsx
+++ b/Leetcode Team 403 Habiter.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC00B2C-6068-4D09-B3FF-18264C8AC419}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6484187-A377-4733-A5F5-80E61D3AD426}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="100">
   <si>
     <t>https://leetcode.com/problems/generate-parentheses/</t>
   </si>
@@ -2072,7 +2072,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K21" sqref="K21"/>
+      <selection pane="bottomRight" activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2402,18 +2402,36 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="12"/>
-      <c r="B19" s="11"/>
+      <c r="B19" s="11">
+        <v>347</v>
+      </c>
       <c r="C19" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
+      <c r="D19" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="12">

</xml_diff>

<commit_message>
problem 22, 33, 378
</commit_message>
<xml_diff>
--- a/Leetcode Team 403 Habiter.xlsx
+++ b/Leetcode Team 403 Habiter.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6484187-A377-4733-A5F5-80E61D3AD426}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F98784-CC0E-4E90-BA08-D8745FE34A8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="100">
   <si>
     <t>https://leetcode.com/problems/generate-parentheses/</t>
   </si>
@@ -388,7 +388,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -411,13 +411,109 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -430,15 +526,263 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="15">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="20" formatCode="dd\-mmm\-yy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -449,6 +793,26 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C260067-204D-4DE0-B389-AD9BBC01A91C}" name="Table1" displayName="Table1" ref="A1:K62" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="13" tableBorderDxfId="14" totalsRowBorderDxfId="12">
+  <autoFilter ref="A1:K62" xr:uid="{116B1116-1037-4952-96B0-4969F8BB6A27}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{D97FE563-CFD8-462C-88F2-C01E4152DEEE}" name="Date" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{E9527249-09A4-424A-BAFE-0E7BC30662E1}" name="Problem #" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{8B765E68-8B4E-4BEF-82B4-EDB9783F6BDF}" name="Problem URL" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{13CD7928-4DED-4779-9896-BC43545F4337}" name="Difficulty" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{67FF5C2A-E60A-4705-9629-45553ABAA771}" name="Done" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{6A1310F5-514C-485B-A587-B9D947B9417F}" name="Top Interviews" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{3AA3576B-9804-4F97-8DD8-FF07619D454D}" name="Most Liked" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{CBC2131C-26DD-4DD7-839B-3C7A594951E8}" name="Amazon" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{72326397-50FB-49F3-B00C-AA3D2AA10575}" name="Facebook" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{E82C2ABA-0938-4BF9-9AF0-AA05E888A695}" name="Google" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{31431F6E-7C6F-4646-8FFD-04F9FD89885E}" name="LinkedIn" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2072,7 +2436,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K19" sqref="K19"/>
+      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2080,42 +2444,46 @@
     <col min="1" max="1" width="13.05078125" customWidth="1"/>
     <col min="2" max="2" width="13.05078125" style="9" customWidth="1"/>
     <col min="3" max="3" width="59.1015625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.20703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.3125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5234375" customWidth="1"/>
+    <col min="6" max="6" width="14.05078125" customWidth="1"/>
+    <col min="7" max="7" width="11.15625" customWidth="1"/>
+    <col min="8" max="8" width="9" customWidth="1"/>
+    <col min="9" max="9" width="10.15625" customWidth="1"/>
+    <col min="11" max="11" width="9.1015625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="17" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2138,7 +2506,7 @@
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
+      <c r="K2" s="13"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="12"/>
@@ -2157,7 +2525,7 @@
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
+      <c r="K3" s="13"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="12">
@@ -2174,7 +2542,7 @@
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
+      <c r="K4" s="13"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="12"/>
@@ -2189,7 +2557,7 @@
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
+      <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="12">
@@ -2206,7 +2574,7 @@
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
+      <c r="K6" s="13"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="12"/>
@@ -2221,7 +2589,7 @@
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
+      <c r="K7" s="13"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="12">
@@ -2238,7 +2606,7 @@
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
+      <c r="K8" s="13"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="12"/>
@@ -2253,14 +2621,14 @@
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
+      <c r="K9" s="13"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="12">
         <v>43956</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="22" t="s">
         <v>76</v>
       </c>
       <c r="D10" s="10"/>
@@ -2270,7 +2638,7 @@
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
+      <c r="K10" s="13"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="12"/>
@@ -2285,7 +2653,7 @@
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
+      <c r="K11" s="13"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="12">
@@ -2302,7 +2670,7 @@
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
+      <c r="K12" s="13"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="12"/>
@@ -2317,14 +2685,14 @@
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
+      <c r="K13" s="13"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="12">
         <v>43958</v>
       </c>
       <c r="B14" s="11"/>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="22" t="s">
         <v>72</v>
       </c>
       <c r="D14" s="10"/>
@@ -2334,7 +2702,7 @@
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
+      <c r="K14" s="13"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="12"/>
@@ -2349,14 +2717,14 @@
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
+      <c r="K15" s="13"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="12">
         <v>43959</v>
       </c>
       <c r="B16" s="11"/>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="22" t="s">
         <v>70</v>
       </c>
       <c r="D16" s="10"/>
@@ -2366,7 +2734,7 @@
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
+      <c r="K16" s="13"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="12"/>
@@ -2381,24 +2749,42 @@
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
+      <c r="K17" s="13"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="12">
         <v>43960</v>
       </c>
-      <c r="B18" s="11"/>
+      <c r="B18" s="11">
+        <v>378</v>
+      </c>
       <c r="C18" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
+      <c r="D18" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="12"/>
@@ -2429,7 +2815,7 @@
       <c r="J19" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="K19" s="10" t="s">
+      <c r="K19" s="13" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2464,7 +2850,7 @@
       <c r="J20" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="K20" s="10" t="s">
+      <c r="K20" s="13" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2497,7 +2883,7 @@
       <c r="J21" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="K21" s="10" t="s">
+      <c r="K21" s="13" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2532,7 +2918,7 @@
       <c r="J22" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="K22" s="10" t="s">
+      <c r="K22" s="13" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2541,7 +2927,7 @@
       <c r="B23" s="11">
         <v>19</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="22" t="s">
         <v>48</v>
       </c>
       <c r="D23" s="10" t="s">
@@ -2565,7 +2951,7 @@
       <c r="J23" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="K23" s="10" t="s">
+      <c r="K23" s="13" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2573,29 +2959,69 @@
       <c r="A24" s="12">
         <v>43963</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
+      <c r="B24" s="11">
+        <v>22</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="J24" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="K24" s="13" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="12"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
+      <c r="B25" s="11">
+        <v>33</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="K25" s="13" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="12">
@@ -2610,7 +3036,7 @@
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
       <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
+      <c r="K26" s="13"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="12"/>
@@ -2623,7 +3049,7 @@
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
+      <c r="K27" s="13"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="12">
@@ -2638,7 +3064,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
       <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
+      <c r="K28" s="13"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="12"/>
@@ -2651,7 +3077,7 @@
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
+      <c r="K29" s="13"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="12">
@@ -2666,7 +3092,7 @@
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
       <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
+      <c r="K30" s="13"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="12"/>
@@ -2679,7 +3105,7 @@
       <c r="H31" s="10"/>
       <c r="I31" s="10"/>
       <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
+      <c r="K31" s="13"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="12">
@@ -2694,7 +3120,7 @@
       <c r="H32" s="10"/>
       <c r="I32" s="10"/>
       <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
+      <c r="K32" s="13"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="12"/>
@@ -2707,7 +3133,7 @@
       <c r="H33" s="10"/>
       <c r="I33" s="10"/>
       <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
+      <c r="K33" s="13"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="12">
@@ -2722,7 +3148,7 @@
       <c r="H34" s="10"/>
       <c r="I34" s="10"/>
       <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
+      <c r="K34" s="13"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="12"/>
@@ -2735,7 +3161,7 @@
       <c r="H35" s="10"/>
       <c r="I35" s="10"/>
       <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
+      <c r="K35" s="13"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="12">
@@ -2750,7 +3176,7 @@
       <c r="H36" s="10"/>
       <c r="I36" s="10"/>
       <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
+      <c r="K36" s="13"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="12"/>
@@ -2763,7 +3189,7 @@
       <c r="H37" s="10"/>
       <c r="I37" s="10"/>
       <c r="J37" s="10"/>
-      <c r="K37" s="10"/>
+      <c r="K37" s="13"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="12">
@@ -2778,7 +3204,7 @@
       <c r="H38" s="10"/>
       <c r="I38" s="10"/>
       <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
+      <c r="K38" s="13"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="12"/>
@@ -2791,7 +3217,7 @@
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
       <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
+      <c r="K39" s="13"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="12">
@@ -2806,7 +3232,7 @@
       <c r="H40" s="10"/>
       <c r="I40" s="10"/>
       <c r="J40" s="10"/>
-      <c r="K40" s="10"/>
+      <c r="K40" s="13"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="12"/>
@@ -2819,7 +3245,7 @@
       <c r="H41" s="10"/>
       <c r="I41" s="10"/>
       <c r="J41" s="10"/>
-      <c r="K41" s="10"/>
+      <c r="K41" s="13"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="12">
@@ -2834,7 +3260,7 @@
       <c r="H42" s="10"/>
       <c r="I42" s="10"/>
       <c r="J42" s="10"/>
-      <c r="K42" s="10"/>
+      <c r="K42" s="13"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="12"/>
@@ -2847,7 +3273,7 @@
       <c r="H43" s="10"/>
       <c r="I43" s="10"/>
       <c r="J43" s="10"/>
-      <c r="K43" s="10"/>
+      <c r="K43" s="13"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="12">
@@ -2862,7 +3288,7 @@
       <c r="H44" s="10"/>
       <c r="I44" s="10"/>
       <c r="J44" s="10"/>
-      <c r="K44" s="10"/>
+      <c r="K44" s="13"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="12"/>
@@ -2875,7 +3301,7 @@
       <c r="H45" s="10"/>
       <c r="I45" s="10"/>
       <c r="J45" s="10"/>
-      <c r="K45" s="10"/>
+      <c r="K45" s="13"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="12">
@@ -2890,7 +3316,7 @@
       <c r="H46" s="10"/>
       <c r="I46" s="10"/>
       <c r="J46" s="10"/>
-      <c r="K46" s="10"/>
+      <c r="K46" s="13"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="12"/>
@@ -2903,7 +3329,7 @@
       <c r="H47" s="10"/>
       <c r="I47" s="10"/>
       <c r="J47" s="10"/>
-      <c r="K47" s="10"/>
+      <c r="K47" s="13"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="12">
@@ -2918,7 +3344,7 @@
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
       <c r="J48" s="10"/>
-      <c r="K48" s="10"/>
+      <c r="K48" s="13"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="12"/>
@@ -2931,7 +3357,7 @@
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
       <c r="J49" s="10"/>
-      <c r="K49" s="10"/>
+      <c r="K49" s="13"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="12">
@@ -2946,7 +3372,7 @@
       <c r="H50" s="10"/>
       <c r="I50" s="10"/>
       <c r="J50" s="10"/>
-      <c r="K50" s="10"/>
+      <c r="K50" s="13"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="12"/>
@@ -2959,7 +3385,7 @@
       <c r="H51" s="10"/>
       <c r="I51" s="10"/>
       <c r="J51" s="10"/>
-      <c r="K51" s="10"/>
+      <c r="K51" s="13"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="12">
@@ -2974,7 +3400,7 @@
       <c r="H52" s="10"/>
       <c r="I52" s="10"/>
       <c r="J52" s="10"/>
-      <c r="K52" s="10"/>
+      <c r="K52" s="13"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="12"/>
@@ -2987,7 +3413,7 @@
       <c r="H53" s="10"/>
       <c r="I53" s="10"/>
       <c r="J53" s="10"/>
-      <c r="K53" s="10"/>
+      <c r="K53" s="13"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="12">
@@ -3002,7 +3428,7 @@
       <c r="H54" s="10"/>
       <c r="I54" s="10"/>
       <c r="J54" s="10"/>
-      <c r="K54" s="10"/>
+      <c r="K54" s="13"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="12"/>
@@ -3015,7 +3441,7 @@
       <c r="H55" s="10"/>
       <c r="I55" s="10"/>
       <c r="J55" s="10"/>
-      <c r="K55" s="10"/>
+      <c r="K55" s="13"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="12">
@@ -3030,7 +3456,7 @@
       <c r="H56" s="10"/>
       <c r="I56" s="10"/>
       <c r="J56" s="10"/>
-      <c r="K56" s="10"/>
+      <c r="K56" s="13"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="12"/>
@@ -3043,7 +3469,7 @@
       <c r="H57" s="10"/>
       <c r="I57" s="10"/>
       <c r="J57" s="10"/>
-      <c r="K57" s="10"/>
+      <c r="K57" s="13"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="12">
@@ -3058,7 +3484,7 @@
       <c r="H58" s="10"/>
       <c r="I58" s="10"/>
       <c r="J58" s="10"/>
-      <c r="K58" s="10"/>
+      <c r="K58" s="13"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="12"/>
@@ -3071,7 +3497,7 @@
       <c r="H59" s="10"/>
       <c r="I59" s="10"/>
       <c r="J59" s="10"/>
-      <c r="K59" s="10"/>
+      <c r="K59" s="13"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="12">
@@ -3086,7 +3512,7 @@
       <c r="H60" s="10"/>
       <c r="I60" s="10"/>
       <c r="J60" s="10"/>
-      <c r="K60" s="10"/>
+      <c r="K60" s="13"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="12"/>
@@ -3099,30 +3525,27 @@
       <c r="H61" s="10"/>
       <c r="I61" s="10"/>
       <c r="J61" s="10"/>
-      <c r="K61" s="10"/>
+      <c r="K61" s="13"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="12">
+      <c r="A62" s="18">
         <v>43982</v>
       </c>
-      <c r="B62" s="11"/>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="10"/>
-      <c r="G62" s="10"/>
-      <c r="H62" s="10"/>
-      <c r="I62" s="10"/>
-      <c r="J62" s="10"/>
-      <c r="K62" s="10"/>
+      <c r="B62" s="19"/>
+      <c r="C62" s="20"/>
+      <c r="D62" s="20"/>
+      <c r="E62" s="20"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="20"/>
+      <c r="H62" s="20"/>
+      <c r="I62" s="20"/>
+      <c r="J62" s="20"/>
+      <c r="K62" s="21"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C14" r:id="rId1" xr:uid="{143FE984-357E-4C57-9511-1156ECFD382D}"/>
-    <hyperlink ref="C16" r:id="rId2" xr:uid="{9A8C35D7-CF75-4694-AD2B-FE65FF1DD953}"/>
-    <hyperlink ref="C10" r:id="rId3" xr:uid="{D88E1F11-E9F8-4FC7-B486-703E761C33DB}"/>
-    <hyperlink ref="C23" r:id="rId4" xr:uid="{0BA771FA-4374-4404-BAEA-E9BB19053119}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
problem 40, 47, 289
</commit_message>
<xml_diff>
--- a/Leetcode Team 403 Habiter.xlsx
+++ b/Leetcode Team 403 Habiter.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C82F404-3D83-46D8-9DD5-8027026EA1F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C519D28B-3BFC-4D4A-850C-0E9BE33DA3E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="March" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="141">
   <si>
     <t>https://leetcode.com/problems/generate-parentheses/</t>
   </si>
@@ -457,7 +457,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -465,13 +465,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -594,10 +606,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -614,8 +627,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="45">
@@ -1671,11 +1686,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D440FBD-B8AE-4249-BDC1-5DAAC739659E}">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2004,18 +2019,36 @@
       <c r="A18" s="4">
         <v>43899</v>
       </c>
-      <c r="B18" s="3"/>
+      <c r="B18" s="3">
+        <v>46</v>
+      </c>
       <c r="C18" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="5"/>
+      <c r="D18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="4"/>
@@ -2036,18 +2069,36 @@
       <c r="A20" s="4">
         <v>43900</v>
       </c>
-      <c r="B20" s="3"/>
+      <c r="B20" s="3">
+        <v>47</v>
+      </c>
       <c r="C20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="5"/>
+      <c r="D20" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="4"/>
@@ -2775,10 +2826,10 @@
   <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C25" sqref="C25"/>
+      <selection pane="bottomRight" activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3802,11 +3853,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9570534-85A5-4387-8641-9D0197BC7F2B}">
   <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B30" sqref="B30:K30"/>
+      <selection pane="bottomRight" activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4266,7 +4317,7 @@
       <c r="B22" s="3">
         <v>15</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="16" t="s">
         <v>46</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -4699,61 +4750,137 @@
       <c r="A38" s="4">
         <v>43970</v>
       </c>
-      <c r="B38" s="3"/>
+      <c r="B38" s="3">
+        <v>289</v>
+      </c>
       <c r="C38" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="5"/>
+      <c r="D38" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="4"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="2" t="s">
+      <c r="B39" s="3">
+        <v>39</v>
+      </c>
+      <c r="C39" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="5"/>
+      <c r="D39" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="4">
         <v>43971</v>
       </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="5"/>
+      <c r="B40" s="3">
+        <v>47</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K40" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="4"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="5"/>
+      <c r="B41" s="3">
+        <v>40</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="4">

</xml_diff>

<commit_message>
problem 2: add two numbers in linked list
</commit_message>
<xml_diff>
--- a/Leetcode Team 403 Habiter.xlsx
+++ b/Leetcode Team 403 Habiter.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C519D28B-3BFC-4D4A-850C-0E9BE33DA3E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3F8294-CFCF-48F7-AFFB-A35BE475D546}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="March" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="141">
   <si>
     <t>https://leetcode.com/problems/generate-parentheses/</t>
   </si>
@@ -610,7 +610,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -628,6 +628,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1362,8 +1365,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C3B79F8F-34A5-48E2-A520-98D48807E864}" name="Table134" displayName="Table134" ref="A1:K65" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="43" tableBorderDxfId="42" totalsRowBorderDxfId="41">
-  <autoFilter ref="A1:K65" xr:uid="{116B1116-1037-4952-96B0-4969F8BB6A27}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C3B79F8F-34A5-48E2-A520-98D48807E864}" name="Table134" displayName="Table134" ref="A1:K63" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="43" tableBorderDxfId="42" totalsRowBorderDxfId="41">
+  <autoFilter ref="A1:K63" xr:uid="{116B1116-1037-4952-96B0-4969F8BB6A27}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{B3E2ABC1-DFE4-41CF-B266-4C6F87E06327}" name="Date" dataDxfId="40"/>
     <tableColumn id="2" xr3:uid="{D852D979-067D-4DC2-A8D3-F58D99FF98BA}" name="Problem #" dataDxfId="39"/>
@@ -1402,8 +1405,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C260067-204D-4DE0-B389-AD9BBC01A91C}" name="Table1" displayName="Table1" ref="A1:K62" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
-  <autoFilter ref="A1:K62" xr:uid="{116B1116-1037-4952-96B0-4969F8BB6A27}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C260067-204D-4DE0-B389-AD9BBC01A91C}" name="Table1" displayName="Table1" ref="A1:K63" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+  <autoFilter ref="A1:K63" xr:uid="{116B1116-1037-4952-96B0-4969F8BB6A27}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{D97FE563-CFD8-462C-88F2-C01E4152DEEE}" name="Date" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{E9527249-09A4-424A-BAFE-0E7BC30662E1}" name="Problem #" dataDxfId="9"/>
@@ -1686,11 +1689,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D440FBD-B8AE-4249-BDC1-5DAAC739659E}">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomRight" activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1745,129 +1748,273 @@
       <c r="A2" s="4">
         <v>43891</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="3">
+        <v>15</v>
+      </c>
       <c r="C2" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4"/>
-      <c r="B3" s="3"/>
+      <c r="B3" s="3">
+        <v>19</v>
+      </c>
       <c r="C3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4">
         <v>43892</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="3">
+        <v>22</v>
+      </c>
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4"/>
-      <c r="B5" s="3"/>
+      <c r="B5" s="3">
+        <v>33</v>
+      </c>
       <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="5"/>
+      <c r="D5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4">
         <v>43893</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="3">
+        <v>34</v>
+      </c>
       <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="5"/>
+      <c r="D6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4"/>
-      <c r="B7" s="3"/>
+      <c r="B7" s="3">
+        <v>46</v>
+      </c>
       <c r="C7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="5"/>
+      <c r="D7" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4">
         <v>43894</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="3">
+        <v>55</v>
+      </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="5"/>
+      <c r="D8" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4"/>
-      <c r="B9" s="3"/>
+      <c r="B9" s="3">
+        <v>48</v>
+      </c>
       <c r="C9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="5"/>
+      <c r="D9" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4">
@@ -2052,18 +2199,36 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="4"/>
-      <c r="B19" s="3"/>
+      <c r="B19" s="3">
+        <v>39</v>
+      </c>
       <c r="C19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="5"/>
+      <c r="D19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="4">
@@ -2102,35 +2267,71 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="4"/>
-      <c r="B21" s="3"/>
+      <c r="B21" s="3">
+        <v>40</v>
+      </c>
       <c r="C21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="5"/>
+      <c r="D21" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="4">
         <v>43901</v>
       </c>
-      <c r="B22" s="3"/>
+      <c r="B22" s="3">
+        <v>2</v>
+      </c>
       <c r="C22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="5"/>
+      <c r="D22" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="4"/>
@@ -2773,45 +2974,27 @@
       <c r="K62" s="5"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="4"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="2" t="s">
+      <c r="A63" s="10"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
-      <c r="I63" s="2"/>
-      <c r="J63" s="2"/>
-      <c r="K63" s="5"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A64" s="4"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
-      <c r="J64" s="2"/>
-      <c r="K64" s="5"/>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" s="4"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="12"/>
-      <c r="D65" s="2"/>
-      <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
-      <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
-      <c r="I65" s="2"/>
-      <c r="J65" s="2"/>
-      <c r="K65" s="5"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="12"/>
+      <c r="H63" s="12"/>
+      <c r="I63" s="12"/>
+      <c r="J63" s="12"/>
+      <c r="K63" s="13"/>
+    </row>
+    <row r="64" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="17"/>
+      <c r="B64" s="18"/>
+    </row>
+    <row r="65" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="17"/>
+      <c r="B65" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2826,10 +3009,10 @@
   <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C54" sqref="C54"/>
+      <selection pane="bottomRight" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3851,13 +4034,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9570534-85A5-4387-8641-9D0197BC7F2B}">
-  <dimension ref="A1:K62"/>
+  <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C39" sqref="C39"/>
+      <selection pane="bottomRight" activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4886,21 +5069,43 @@
       <c r="A42" s="4">
         <v>43972</v>
       </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="5"/>
+      <c r="B42" s="3">
+        <v>2</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="4"/>
       <c r="B43" s="3"/>
-      <c r="C43" s="2"/>
+      <c r="C43" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
@@ -5177,6 +5382,19 @@
       <c r="J62" s="12"/>
       <c r="K62" s="13"/>
     </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="10"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="12"/>
+      <c r="H63" s="12"/>
+      <c r="I63" s="12"/>
+      <c r="J63" s="12"/>
+      <c r="K63" s="13"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
problem 3 using dictionary and a pointer at the start of the current substring.
</commit_message>
<xml_diff>
--- a/Leetcode Team 403 Habiter.xlsx
+++ b/Leetcode Team 403 Habiter.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3F8294-CFCF-48F7-AFFB-A35BE475D546}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC5B9D0-2945-40E5-808D-FBF3DAB9C8F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="March" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="141">
   <si>
     <t>https://leetcode.com/problems/generate-parentheses/</t>
   </si>
@@ -1689,11 +1689,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D440FBD-B8AE-4249-BDC1-5DAAC739659E}">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H68" sqref="H68"/>
+      <selection pane="bottomRight" activeCell="C23" sqref="B23:K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2335,18 +2335,36 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="4"/>
-      <c r="B23" s="3"/>
+      <c r="B23" s="3">
+        <v>3</v>
+      </c>
       <c r="C23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="5"/>
+      <c r="D23" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="4">
@@ -3009,7 +3027,7 @@
   <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="C37" sqref="C37"/>
@@ -4036,11 +4054,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9570534-85A5-4387-8641-9D0197BC7F2B}">
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C69" sqref="C69"/>
+      <selection pane="bottomRight" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5102,18 +5120,36 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="4"/>
-      <c r="B43" s="3"/>
+      <c r="B43" s="3">
+        <v>3</v>
+      </c>
       <c r="C43" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="5"/>
+      <c r="D43" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K43" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="4">

</xml_diff>

<commit_message>
problem 11 max area using two pointers.
</commit_message>
<xml_diff>
--- a/Leetcode Team 403 Habiter.xlsx
+++ b/Leetcode Team 403 Habiter.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC5B9D0-2945-40E5-808D-FBF3DAB9C8F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0D4990-1FCC-46AC-8350-B167C5BF8A6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="March" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="141">
   <si>
     <t>https://leetcode.com/problems/generate-parentheses/</t>
   </si>
@@ -1689,11 +1689,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D440FBD-B8AE-4249-BDC1-5DAAC739659E}">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="B23:K23"/>
+      <selection pane="bottomRight" activeCell="B25" sqref="B25:K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2385,18 +2385,36 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="4"/>
-      <c r="B25" s="3"/>
+      <c r="B25" s="3">
+        <v>11</v>
+      </c>
       <c r="C25" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="5"/>
+      <c r="D25" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="4">
@@ -4054,11 +4072,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9570534-85A5-4387-8641-9D0197BC7F2B}">
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C43" sqref="C43"/>
+      <selection pane="bottomRight" activeCell="B45" sqref="B45:K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5156,7 +5174,9 @@
         <v>43973</v>
       </c>
       <c r="B44" s="3"/>
-      <c r="C44" s="2"/>
+      <c r="C44" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
@@ -5168,16 +5188,36 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="4"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="5"/>
+      <c r="B45" s="3">
+        <v>11</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K45" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="4">

</xml_diff>

<commit_message>
problem 165 using itertools.zip_longest with fillvalue argument.
</commit_message>
<xml_diff>
--- a/Leetcode Team 403 Habiter.xlsx
+++ b/Leetcode Team 403 Habiter.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0D4990-1FCC-46AC-8350-B167C5BF8A6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF791BA-76C7-401A-B9C3-9D018EFAF987}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="March" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="141">
   <si>
     <t>https://leetcode.com/problems/generate-parentheses/</t>
   </si>
@@ -1689,11 +1689,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D440FBD-B8AE-4249-BDC1-5DAAC739659E}">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B25" sqref="B25:K25"/>
+      <selection pane="bottomRight" activeCell="B17" sqref="B17:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2149,18 +2149,36 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="4"/>
-      <c r="B17" s="3"/>
+      <c r="B17" s="3">
+        <v>79</v>
+      </c>
       <c r="C17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="5"/>
+      <c r="D17" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="4">
@@ -4072,11 +4090,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9570534-85A5-4387-8641-9D0197BC7F2B}">
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B45" sqref="B45:K45"/>
+      <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
problem 334 simple comparisons while iterating over the list.
</commit_message>
<xml_diff>
--- a/Leetcode Team 403 Habiter.xlsx
+++ b/Leetcode Team 403 Habiter.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF791BA-76C7-401A-B9C3-9D018EFAF987}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C799548-38F0-44A0-98BB-9B7C3A1C1FF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="March" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="143">
   <si>
     <t>https://leetcode.com/problems/generate-parentheses/</t>
   </si>
@@ -451,6 +451,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/game-of-life/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/kth-largest-element-in-an-array/discuss/60294/Solution-explained</t>
+  </si>
+  <si>
+    <t>Column1</t>
   </si>
 </sst>
 </file>
@@ -636,7 +642,25 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="46">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1365,60 +1389,58 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C3B79F8F-34A5-48E2-A520-98D48807E864}" name="Table134" displayName="Table134" ref="A1:K63" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="43" tableBorderDxfId="42" totalsRowBorderDxfId="41">
-  <autoFilter ref="A1:K63" xr:uid="{116B1116-1037-4952-96B0-4969F8BB6A27}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C3B79F8F-34A5-48E2-A520-98D48807E864}" name="Table134" displayName="Table134" ref="A1:K63" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44" tableBorderDxfId="43" totalsRowBorderDxfId="42">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B3E2ABC1-DFE4-41CF-B266-4C6F87E06327}" name="Date" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{D852D979-067D-4DC2-A8D3-F58D99FF98BA}" name="Problem #" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{7025E5D3-672C-4FA4-9F3F-E1B647279073}" name="Problem URL" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{F81AD9F7-6969-4C1D-82AF-E46E2DBC2668}" name="Difficulty" dataDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{4C6862D0-7D2B-4C62-BB99-B3A2CEC64A5E}" name="Solved" dataDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{72FF14F9-0236-434D-B7BC-F119041A3858}" name="Top Interviews" dataDxfId="35"/>
-    <tableColumn id="7" xr3:uid="{5C9B7229-C348-4A10-B7A7-1210D9FE0C0E}" name="Most Liked" dataDxfId="34"/>
-    <tableColumn id="8" xr3:uid="{94F9A000-47E5-4228-B070-3B2C13EB1AD1}" name="Amazon" dataDxfId="33"/>
-    <tableColumn id="9" xr3:uid="{92B0E2A3-76A8-4549-AA5D-108B4D679B77}" name="Facebook" dataDxfId="32"/>
-    <tableColumn id="10" xr3:uid="{6671C8FE-33F8-4C38-A35D-F4FF9BADAEC6}" name="Google" dataDxfId="31"/>
-    <tableColumn id="11" xr3:uid="{A31E59BF-042F-4790-B8E4-E936BED59AA3}" name="LinkedIn" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{B3E2ABC1-DFE4-41CF-B266-4C6F87E06327}" name="Date" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{D852D979-067D-4DC2-A8D3-F58D99FF98BA}" name="Problem #" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{7025E5D3-672C-4FA4-9F3F-E1B647279073}" name="Problem URL" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{F81AD9F7-6969-4C1D-82AF-E46E2DBC2668}" name="Difficulty" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{4C6862D0-7D2B-4C62-BB99-B3A2CEC64A5E}" name="Solved" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{72FF14F9-0236-434D-B7BC-F119041A3858}" name="Top Interviews" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{5C9B7229-C348-4A10-B7A7-1210D9FE0C0E}" name="Most Liked" dataDxfId="35"/>
+    <tableColumn id="8" xr3:uid="{94F9A000-47E5-4228-B070-3B2C13EB1AD1}" name="Amazon" dataDxfId="34"/>
+    <tableColumn id="9" xr3:uid="{92B0E2A3-76A8-4549-AA5D-108B4D679B77}" name="Facebook" dataDxfId="33"/>
+    <tableColumn id="10" xr3:uid="{6671C8FE-33F8-4C38-A35D-F4FF9BADAEC6}" name="Google" dataDxfId="32"/>
+    <tableColumn id="11" xr3:uid="{A31E59BF-042F-4790-B8E4-E936BED59AA3}" name="LinkedIn" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0549819D-3D5F-48EB-A65F-025354882917}" name="Table13" displayName="Table13" ref="A1:K61" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
-  <autoFilter ref="A1:K61" xr:uid="{116B1116-1037-4952-96B0-4969F8BB6A27}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0549819D-3D5F-48EB-A65F-025354882917}" name="Table13" displayName="Table13" ref="A1:K61" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{5CDA05DB-5000-4C00-A633-66BF5622D6CD}" name="Date" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{7C6B0860-8335-48BD-B7C1-AFB62305E598}" name="Problem #" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{FC1AE57B-B991-45CD-9BA8-367D5D66DDFC}" name="Problem URL" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{7B9C4890-7028-4D2D-A735-93498BD634DD}" name="Difficulty" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{A1BFF24E-EC8F-4F1D-8F03-8F7B483DFB42}" name="Solved" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{195096CE-0E6A-414C-BC23-FC23890423A9}" name="Top Interviews" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{F0378ED8-CEEC-4E8E-BC9E-913A13A9AFFE}" name="Most Liked" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{0F66337C-7A88-4842-A889-3BD5E7F7082C}" name="Amazon" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{DEEF1C30-00D2-4B87-8A0F-96FA04079885}" name="Facebook" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{35C548D7-8613-4025-A49A-A1997303F552}" name="Google" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{D67985E4-DC76-475C-84B3-CA05145CF3C9}" name="LinkedIn" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{5CDA05DB-5000-4C00-A633-66BF5622D6CD}" name="Date" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{7C6B0860-8335-48BD-B7C1-AFB62305E598}" name="Problem #" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{FC1AE57B-B991-45CD-9BA8-367D5D66DDFC}" name="Problem URL" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{7B9C4890-7028-4D2D-A735-93498BD634DD}" name="Difficulty" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{A1BFF24E-EC8F-4F1D-8F03-8F7B483DFB42}" name="Solved" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{195096CE-0E6A-414C-BC23-FC23890423A9}" name="Top Interviews" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{F0378ED8-CEEC-4E8E-BC9E-913A13A9AFFE}" name="Most Liked" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{0F66337C-7A88-4842-A889-3BD5E7F7082C}" name="Amazon" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{DEEF1C30-00D2-4B87-8A0F-96FA04079885}" name="Facebook" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{35C548D7-8613-4025-A49A-A1997303F552}" name="Google" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{D67985E4-DC76-475C-84B3-CA05145CF3C9}" name="LinkedIn" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C260067-204D-4DE0-B389-AD9BBC01A91C}" name="Table1" displayName="Table1" ref="A1:K63" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
-  <autoFilter ref="A1:K63" xr:uid="{116B1116-1037-4952-96B0-4969F8BB6A27}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{D97FE563-CFD8-462C-88F2-C01E4152DEEE}" name="Date" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{E9527249-09A4-424A-BAFE-0E7BC30662E1}" name="Problem #" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{8B765E68-8B4E-4BEF-82B4-EDB9783F6BDF}" name="Problem URL" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{13CD7928-4DED-4779-9896-BC43545F4337}" name="Difficulty" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{67FF5C2A-E60A-4705-9629-45553ABAA771}" name="Done" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{6A1310F5-514C-485B-A587-B9D947B9417F}" name="Top Interviews" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{3AA3576B-9804-4F97-8DD8-FF07619D454D}" name="Most Liked" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{CBC2131C-26DD-4DD7-839B-3C7A594951E8}" name="Amazon" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{72326397-50FB-49F3-B00C-AA3D2AA10575}" name="Facebook" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{E82C2ABA-0938-4BF9-9AF0-AA05E888A695}" name="Google" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{31431F6E-7C6F-4646-8FFD-04F9FD89885E}" name="LinkedIn" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C260067-204D-4DE0-B389-AD9BBC01A91C}" name="Table1" displayName="Table1" ref="A1:L63" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{D97FE563-CFD8-462C-88F2-C01E4152DEEE}" name="Date" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{E9527249-09A4-424A-BAFE-0E7BC30662E1}" name="Problem #" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{8B765E68-8B4E-4BEF-82B4-EDB9783F6BDF}" name="Problem URL" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{13CD7928-4DED-4779-9896-BC43545F4337}" name="Difficulty" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{67FF5C2A-E60A-4705-9629-45553ABAA771}" name="Done" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{6A1310F5-514C-485B-A587-B9D947B9417F}" name="Top Interviews" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{3AA3576B-9804-4F97-8DD8-FF07619D454D}" name="Most Liked" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{CBC2131C-26DD-4DD7-839B-3C7A594951E8}" name="Amazon" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{72326397-50FB-49F3-B00C-AA3D2AA10575}" name="Facebook" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{E82C2ABA-0938-4BF9-9AF0-AA05E888A695}" name="Google" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{31431F6E-7C6F-4646-8FFD-04F9FD89885E}" name="LinkedIn" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{946FB028-E4E2-424E-93DA-304146C527C2}" name="Column1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1690,10 +1712,10 @@
   <dimension ref="A1:K65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B17" sqref="B17:K17"/>
+      <selection pane="bottomRight" activeCell="B32" sqref="B32:K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2534,18 +2556,36 @@
       <c r="A32" s="4">
         <v>43906</v>
       </c>
-      <c r="B32" s="3"/>
+      <c r="B32" s="3">
+        <v>334</v>
+      </c>
       <c r="C32" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="5"/>
+      <c r="D32" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K32" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="4"/>
@@ -3063,10 +3103,10 @@
   <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C37" sqref="C37"/>
+      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4088,13 +4128,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9570534-85A5-4387-8641-9D0197BC7F2B}">
-  <dimension ref="A1:K63"/>
+  <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
+      <selection pane="bottomRight" activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4110,7 +4150,7 @@
     <col min="11" max="11" width="9.1015625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>82</v>
       </c>
@@ -4144,8 +4184,11 @@
       <c r="K1" s="9" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L1" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4">
         <v>43952</v>
       </c>
@@ -4165,8 +4208,9 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="5"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L2" s="8"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4"/>
       <c r="B3" s="3">
         <v>151</v>
@@ -4184,8 +4228,9 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="5"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4">
         <v>43953</v>
       </c>
@@ -4201,8 +4246,9 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="5"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4"/>
       <c r="B5" s="3"/>
       <c r="C5" s="2" t="s">
@@ -4216,8 +4262,9 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="5"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4">
         <v>43954</v>
       </c>
@@ -4233,8 +4280,9 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="5"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4"/>
       <c r="B7" s="3"/>
       <c r="C7" s="2" t="s">
@@ -4248,8 +4296,9 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="5"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4">
         <v>43955</v>
       </c>
@@ -4265,8 +4314,9 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="5"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4"/>
       <c r="B9" s="3"/>
       <c r="C9" s="2" t="s">
@@ -4280,8 +4330,9 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="5"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4">
         <v>43956</v>
       </c>
@@ -4297,8 +4348,9 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="5"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4"/>
       <c r="B11" s="3"/>
       <c r="C11" s="2" t="s">
@@ -4312,8 +4364,9 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="5"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="4">
         <v>43957</v>
       </c>
@@ -4329,8 +4382,9 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="5"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="4"/>
       <c r="B13" s="3"/>
       <c r="C13" s="2" t="s">
@@ -4344,8 +4398,9 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="5"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="4">
         <v>43958</v>
       </c>
@@ -4361,8 +4416,9 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="4"/>
       <c r="B15" s="3"/>
       <c r="C15" s="2" t="s">
@@ -4376,8 +4432,9 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="5"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="4">
         <v>43959</v>
       </c>
@@ -4393,8 +4450,9 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="5"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="4"/>
       <c r="B17" s="3"/>
       <c r="C17" s="2" t="s">
@@ -4410,8 +4468,9 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="5"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="4">
         <v>43960</v>
       </c>
@@ -4445,8 +4504,9 @@
       <c r="K18" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="4"/>
       <c r="B19" s="3">
         <v>347</v>
@@ -4478,8 +4538,9 @@
       <c r="K19" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="4">
         <v>43961</v>
       </c>
@@ -4513,8 +4574,9 @@
       <c r="K20" s="5" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="4"/>
       <c r="B21" s="3">
         <v>131</v>
@@ -4546,8 +4608,9 @@
       <c r="K21" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="4">
         <v>43962</v>
       </c>
@@ -4581,8 +4644,9 @@
       <c r="K22" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="4"/>
       <c r="B23" s="3">
         <v>19</v>
@@ -4614,8 +4678,9 @@
       <c r="K23" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="4">
         <v>43963</v>
       </c>
@@ -4649,8 +4714,9 @@
       <c r="K24" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="4"/>
       <c r="B25" s="3">
         <v>33</v>
@@ -4682,8 +4748,9 @@
       <c r="K25" s="5" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="4">
         <v>43964</v>
       </c>
@@ -4717,8 +4784,9 @@
       <c r="K26" s="5" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="4"/>
       <c r="B27" s="3">
         <v>46</v>
@@ -4750,8 +4818,9 @@
       <c r="K27" s="5" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="4">
         <v>43965</v>
       </c>
@@ -4785,8 +4854,9 @@
       <c r="K28" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="4"/>
       <c r="B29" s="3">
         <v>55</v>
@@ -4818,8 +4888,9 @@
       <c r="K29" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="4">
         <v>43966</v>
       </c>
@@ -4853,8 +4924,9 @@
       <c r="K30" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="4"/>
       <c r="B31" s="3"/>
       <c r="C31" s="2" t="s">
@@ -4868,8 +4940,9 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="5"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="4">
         <v>43967</v>
       </c>
@@ -4885,8 +4958,9 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="5"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="4"/>
       <c r="B33" s="3"/>
       <c r="C33" s="2" t="s">
@@ -4900,8 +4974,9 @@
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="5"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="4">
         <v>43968</v>
       </c>
@@ -4917,8 +4992,9 @@
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="5"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="4"/>
       <c r="B35" s="3"/>
       <c r="C35" s="2" t="s">
@@ -4932,8 +5008,9 @@
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="5"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="4">
         <v>43969</v>
       </c>
@@ -4949,8 +5026,9 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="5"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="4"/>
       <c r="B37" s="3">
         <v>79</v>
@@ -4982,8 +5060,9 @@
       <c r="K37" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="4">
         <v>43970</v>
       </c>
@@ -5017,8 +5096,9 @@
       <c r="K38" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="4"/>
       <c r="B39" s="3">
         <v>39</v>
@@ -5050,8 +5130,9 @@
       <c r="K39" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="4">
         <v>43971</v>
       </c>
@@ -5085,8 +5166,9 @@
       <c r="K40" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="4"/>
       <c r="B41" s="3">
         <v>40</v>
@@ -5118,8 +5200,9 @@
       <c r="K41" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="4">
         <v>43972</v>
       </c>
@@ -5153,8 +5236,9 @@
       <c r="K42" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="4"/>
       <c r="B43" s="3">
         <v>3</v>
@@ -5186,8 +5270,9 @@
       <c r="K43" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="4">
         <v>43973</v>
       </c>
@@ -5203,8 +5288,9 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="5"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L44" s="2"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="4"/>
       <c r="B45" s="3">
         <v>11</v>
@@ -5236,13 +5322,16 @@
       <c r="K45" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L45" s="2"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="4">
         <v>43974</v>
       </c>
       <c r="B46" s="3"/>
-      <c r="C46" s="2"/>
+      <c r="C46" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
@@ -5251,11 +5340,16 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="5"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L46" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="4"/>
       <c r="B47" s="3"/>
-      <c r="C47" s="2"/>
+      <c r="C47" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
@@ -5264,13 +5358,16 @@
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="5"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L47" s="2"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="4">
         <v>43975</v>
       </c>
       <c r="B48" s="3"/>
-      <c r="C48" s="2"/>
+      <c r="C48" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
@@ -5279,11 +5376,14 @@
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="5"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L48" s="2"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="4"/>
       <c r="B49" s="3"/>
-      <c r="C49" s="2"/>
+      <c r="C49" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
@@ -5292,13 +5392,16 @@
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="5"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L49" s="2"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="4">
         <v>43976</v>
       </c>
       <c r="B50" s="3"/>
-      <c r="C50" s="2"/>
+      <c r="C50" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
@@ -5307,11 +5410,14 @@
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="5"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L50" s="2"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="4"/>
       <c r="B51" s="3"/>
-      <c r="C51" s="2"/>
+      <c r="C51" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
@@ -5320,26 +5426,50 @@
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="5"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L51" s="2"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="4">
         <v>43977</v>
       </c>
-      <c r="B52" s="3"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="5"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B52" s="3">
+        <v>334</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K52" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L52" s="2"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="4"/>
       <c r="B53" s="3"/>
-      <c r="C53" s="2"/>
+      <c r="C53" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
@@ -5348,8 +5478,9 @@
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="5"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L53" s="2"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="4">
         <v>43978</v>
       </c>
@@ -5363,8 +5494,9 @@
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="5"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L54" s="2"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="4"/>
       <c r="B55" s="3"/>
       <c r="C55" s="2"/>
@@ -5376,8 +5508,9 @@
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="5"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L55" s="2"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="4">
         <v>43979</v>
       </c>
@@ -5391,8 +5524,9 @@
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
       <c r="K56" s="5"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L56" s="2"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="4"/>
       <c r="B57" s="3"/>
       <c r="C57" s="2"/>
@@ -5404,8 +5538,9 @@
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
       <c r="K57" s="5"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L57" s="2"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="4">
         <v>43980</v>
       </c>
@@ -5419,8 +5554,9 @@
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
       <c r="K58" s="5"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L58" s="2"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="4"/>
       <c r="B59" s="3"/>
       <c r="C59" s="2"/>
@@ -5432,8 +5568,9 @@
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
       <c r="K59" s="5"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L59" s="2"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="4">
         <v>43981</v>
       </c>
@@ -5447,8 +5584,9 @@
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
       <c r="K60" s="5"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L60" s="2"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="4"/>
       <c r="B61" s="3"/>
       <c r="C61" s="2"/>
@@ -5460,8 +5598,9 @@
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
       <c r="K61" s="5"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L61" s="2"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="10">
         <v>43982</v>
       </c>
@@ -5475,8 +5614,9 @@
       <c r="I62" s="12"/>
       <c r="J62" s="12"/>
       <c r="K62" s="13"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L62" s="2"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="10"/>
       <c r="B63" s="11"/>
       <c r="C63" s="12"/>
@@ -5488,6 +5628,7 @@
       <c r="I63" s="12"/>
       <c r="J63" s="12"/>
       <c r="K63" s="13"/>
+      <c r="L63" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
problem 54 spiral matrix. Simple array traversal manipulation.
</commit_message>
<xml_diff>
--- a/Leetcode Team 403 Habiter.xlsx
+++ b/Leetcode Team 403 Habiter.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C799548-38F0-44A0-98BB-9B7C3A1C1FF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9068C32C-829A-4FDA-A4B2-1592BA008133}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="143">
   <si>
     <t>https://leetcode.com/problems/generate-parentheses/</t>
   </si>
@@ -1722,7 +1722,7 @@
   <cols>
     <col min="1" max="1" width="13.05078125" customWidth="1"/>
     <col min="2" max="2" width="13.05078125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="69.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.47265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5234375" customWidth="1"/>
     <col min="6" max="6" width="14.05078125" customWidth="1"/>
     <col min="7" max="7" width="11.15625" customWidth="1"/>
@@ -4131,17 +4131,17 @@
   <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C56" sqref="C56"/>
+      <selection pane="bottomRight" activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="13.05078125" customWidth="1"/>
     <col min="2" max="2" width="13.05078125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="69.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.47265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5234375" customWidth="1"/>
     <col min="6" max="6" width="14.05078125" customWidth="1"/>
     <col min="7" max="7" width="11.15625" customWidth="1"/>
@@ -5485,7 +5485,9 @@
         <v>43978</v>
       </c>
       <c r="B54" s="3"/>
-      <c r="C54" s="2"/>
+      <c r="C54" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
@@ -5499,7 +5501,9 @@
     <row r="55" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="4"/>
       <c r="B55" s="3"/>
-      <c r="C55" s="2"/>
+      <c r="C55" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>

</xml_diff>

<commit_message>
problem 328 odd and even items in the linked list are unshuffled into two lists.
</commit_message>
<xml_diff>
--- a/Leetcode Team 403 Habiter.xlsx
+++ b/Leetcode Team 403 Habiter.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9068C32C-829A-4FDA-A4B2-1592BA008133}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E170FC5C-2398-41EA-B8F7-74B033B8E3FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,6 +11,7 @@
     <sheet name="March" sheetId="5" r:id="rId1"/>
     <sheet name="April" sheetId="4" r:id="rId2"/>
     <sheet name="May" sheetId="3" r:id="rId3"/>
+    <sheet name="June" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="148">
   <si>
     <t>https://leetcode.com/problems/generate-parentheses/</t>
   </si>
@@ -457,6 +458,21 @@
   </si>
   <si>
     <t>Column1</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/friend-circles/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/trapping-rain-water/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-substrings-between-each-pair-of-parentheses/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-remove-to-make-valid-parentheses/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/flatten-a-multilevel-doubly-linked-list/</t>
   </si>
 </sst>
 </file>
@@ -616,7 +632,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -637,12 +653,269 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="46">
+  <dxfs count="62">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="20" formatCode="dd\-mmm\-yy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1389,58 +1662,78 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C3B79F8F-34A5-48E2-A520-98D48807E864}" name="Table134" displayName="Table134" ref="A1:K63" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C3B79F8F-34A5-48E2-A520-98D48807E864}" name="Table134" displayName="Table134" ref="A1:K63" totalsRowShown="0" headerRowDxfId="61" headerRowBorderDxfId="60" tableBorderDxfId="59" totalsRowBorderDxfId="58">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B3E2ABC1-DFE4-41CF-B266-4C6F87E06327}" name="Date" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{D852D979-067D-4DC2-A8D3-F58D99FF98BA}" name="Problem #" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{7025E5D3-672C-4FA4-9F3F-E1B647279073}" name="Problem URL" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{F81AD9F7-6969-4C1D-82AF-E46E2DBC2668}" name="Difficulty" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{4C6862D0-7D2B-4C62-BB99-B3A2CEC64A5E}" name="Solved" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{72FF14F9-0236-434D-B7BC-F119041A3858}" name="Top Interviews" dataDxfId="36"/>
-    <tableColumn id="7" xr3:uid="{5C9B7229-C348-4A10-B7A7-1210D9FE0C0E}" name="Most Liked" dataDxfId="35"/>
-    <tableColumn id="8" xr3:uid="{94F9A000-47E5-4228-B070-3B2C13EB1AD1}" name="Amazon" dataDxfId="34"/>
-    <tableColumn id="9" xr3:uid="{92B0E2A3-76A8-4549-AA5D-108B4D679B77}" name="Facebook" dataDxfId="33"/>
-    <tableColumn id="10" xr3:uid="{6671C8FE-33F8-4C38-A35D-F4FF9BADAEC6}" name="Google" dataDxfId="32"/>
-    <tableColumn id="11" xr3:uid="{A31E59BF-042F-4790-B8E4-E936BED59AA3}" name="LinkedIn" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{B3E2ABC1-DFE4-41CF-B266-4C6F87E06327}" name="Date" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{D852D979-067D-4DC2-A8D3-F58D99FF98BA}" name="Problem #" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{7025E5D3-672C-4FA4-9F3F-E1B647279073}" name="Problem URL" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{F81AD9F7-6969-4C1D-82AF-E46E2DBC2668}" name="Difficulty" dataDxfId="54"/>
+    <tableColumn id="5" xr3:uid="{4C6862D0-7D2B-4C62-BB99-B3A2CEC64A5E}" name="Solved" dataDxfId="53"/>
+    <tableColumn id="6" xr3:uid="{72FF14F9-0236-434D-B7BC-F119041A3858}" name="Top Interviews" dataDxfId="52"/>
+    <tableColumn id="7" xr3:uid="{5C9B7229-C348-4A10-B7A7-1210D9FE0C0E}" name="Most Liked" dataDxfId="51"/>
+    <tableColumn id="8" xr3:uid="{94F9A000-47E5-4228-B070-3B2C13EB1AD1}" name="Amazon" dataDxfId="50"/>
+    <tableColumn id="9" xr3:uid="{92B0E2A3-76A8-4549-AA5D-108B4D679B77}" name="Facebook" dataDxfId="49"/>
+    <tableColumn id="10" xr3:uid="{6671C8FE-33F8-4C38-A35D-F4FF9BADAEC6}" name="Google" dataDxfId="48"/>
+    <tableColumn id="11" xr3:uid="{A31E59BF-042F-4790-B8E4-E936BED59AA3}" name="LinkedIn" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0549819D-3D5F-48EB-A65F-025354882917}" name="Table13" displayName="Table13" ref="A1:K61" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0549819D-3D5F-48EB-A65F-025354882917}" name="Table13" displayName="Table13" ref="A1:K61" totalsRowShown="0" headerRowDxfId="46" headerRowBorderDxfId="45" tableBorderDxfId="44" totalsRowBorderDxfId="43">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{5CDA05DB-5000-4C00-A633-66BF5622D6CD}" name="Date" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{7C6B0860-8335-48BD-B7C1-AFB62305E598}" name="Problem #" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{FC1AE57B-B991-45CD-9BA8-367D5D66DDFC}" name="Problem URL" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{7B9C4890-7028-4D2D-A735-93498BD634DD}" name="Difficulty" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{A1BFF24E-EC8F-4F1D-8F03-8F7B483DFB42}" name="Solved" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{195096CE-0E6A-414C-BC23-FC23890423A9}" name="Top Interviews" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{F0378ED8-CEEC-4E8E-BC9E-913A13A9AFFE}" name="Most Liked" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{0F66337C-7A88-4842-A889-3BD5E7F7082C}" name="Amazon" dataDxfId="19"/>
-    <tableColumn id="9" xr3:uid="{DEEF1C30-00D2-4B87-8A0F-96FA04079885}" name="Facebook" dataDxfId="18"/>
-    <tableColumn id="10" xr3:uid="{35C548D7-8613-4025-A49A-A1997303F552}" name="Google" dataDxfId="17"/>
-    <tableColumn id="11" xr3:uid="{D67985E4-DC76-475C-84B3-CA05145CF3C9}" name="LinkedIn" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{5CDA05DB-5000-4C00-A633-66BF5622D6CD}" name="Date" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{7C6B0860-8335-48BD-B7C1-AFB62305E598}" name="Problem #" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{FC1AE57B-B991-45CD-9BA8-367D5D66DDFC}" name="Problem URL" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{7B9C4890-7028-4D2D-A735-93498BD634DD}" name="Difficulty" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{A1BFF24E-EC8F-4F1D-8F03-8F7B483DFB42}" name="Solved" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{195096CE-0E6A-414C-BC23-FC23890423A9}" name="Top Interviews" dataDxfId="37"/>
+    <tableColumn id="7" xr3:uid="{F0378ED8-CEEC-4E8E-BC9E-913A13A9AFFE}" name="Most Liked" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{0F66337C-7A88-4842-A889-3BD5E7F7082C}" name="Amazon" dataDxfId="35"/>
+    <tableColumn id="9" xr3:uid="{DEEF1C30-00D2-4B87-8A0F-96FA04079885}" name="Facebook" dataDxfId="34"/>
+    <tableColumn id="10" xr3:uid="{35C548D7-8613-4025-A49A-A1997303F552}" name="Google" dataDxfId="33"/>
+    <tableColumn id="11" xr3:uid="{D67985E4-DC76-475C-84B3-CA05145CF3C9}" name="LinkedIn" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C260067-204D-4DE0-B389-AD9BBC01A91C}" name="Table1" displayName="Table1" ref="A1:L63" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C260067-204D-4DE0-B389-AD9BBC01A91C}" name="Table1" displayName="Table1" ref="A1:L63" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{D97FE563-CFD8-462C-88F2-C01E4152DEEE}" name="Date" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{E9527249-09A4-424A-BAFE-0E7BC30662E1}" name="Problem #" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{8B765E68-8B4E-4BEF-82B4-EDB9783F6BDF}" name="Problem URL" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{13CD7928-4DED-4779-9896-BC43545F4337}" name="Difficulty" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{67FF5C2A-E60A-4705-9629-45553ABAA771}" name="Done" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{6A1310F5-514C-485B-A587-B9D947B9417F}" name="Top Interviews" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{3AA3576B-9804-4F97-8DD8-FF07619D454D}" name="Most Liked" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{CBC2131C-26DD-4DD7-839B-3C7A594951E8}" name="Amazon" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{72326397-50FB-49F3-B00C-AA3D2AA10575}" name="Facebook" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{E82C2ABA-0938-4BF9-9AF0-AA05E888A695}" name="Google" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{31431F6E-7C6F-4646-8FFD-04F9FD89885E}" name="LinkedIn" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{946FB028-E4E2-424E-93DA-304146C527C2}" name="Column1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{D97FE563-CFD8-462C-88F2-C01E4152DEEE}" name="Date" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{E9527249-09A4-424A-BAFE-0E7BC30662E1}" name="Problem #" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{8B765E68-8B4E-4BEF-82B4-EDB9783F6BDF}" name="Problem URL" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{13CD7928-4DED-4779-9896-BC43545F4337}" name="Difficulty" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{67FF5C2A-E60A-4705-9629-45553ABAA771}" name="Done" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{6A1310F5-514C-485B-A587-B9D947B9417F}" name="Top Interviews" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{3AA3576B-9804-4F97-8DD8-FF07619D454D}" name="Most Liked" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{CBC2131C-26DD-4DD7-839B-3C7A594951E8}" name="Amazon" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{72326397-50FB-49F3-B00C-AA3D2AA10575}" name="Facebook" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{E82C2ABA-0938-4BF9-9AF0-AA05E888A695}" name="Google" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{31431F6E-7C6F-4646-8FFD-04F9FD89885E}" name="LinkedIn" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{946FB028-E4E2-424E-93DA-304146C527C2}" name="Column1" dataDxfId="16"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{34A5C7DE-E003-42F0-8FBE-3B98000334D8}" name="Table15" displayName="Table15" ref="A1:L61" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="13" tableBorderDxfId="14" totalsRowBorderDxfId="12">
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{A58CB880-41C7-4BDB-8A45-ACC4023CC087}" name="Date" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{C810554A-0AF3-4476-9084-1B8403573491}" name="Problem #" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{AE2548DB-F43F-4407-994C-C76E1C1015FE}" name="Problem URL" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{A55650E6-6475-48D6-9E1B-A53C50341856}" name="Difficulty" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{5BEC5DBF-C271-419C-8FF5-0BE151B16BC5}" name="Done" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{AEAE9C99-0023-4D64-8E36-4A81A1AAC3FB}" name="Top Interviews" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{41C684E6-D890-4F04-A167-9EB05CE52736}" name="Most Liked" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{D655B86E-CC8C-4581-A99E-946DC2107E3D}" name="Amazon" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{EDF1F749-934C-4AB3-B815-B4DB9E44725D}" name="Facebook" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{D4D114EB-F41E-418A-856F-EDC352E8854D}" name="Google" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{2666CAFC-3B33-4EBB-9A51-AD9CA119EDB5}" name="LinkedIn" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{7635171E-8EC8-436F-9264-9973B50380B5}" name="Column1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4131,10 +4424,10 @@
   <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C55" sqref="C55"/>
+      <selection pane="bottomRight" activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5519,6 +5812,1078 @@
         <v>43979</v>
       </c>
       <c r="B56" s="3"/>
+      <c r="C56" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="2"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="4"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="5"/>
+      <c r="L57" s="2"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="4">
+        <v>43980</v>
+      </c>
+      <c r="B58" s="3"/>
+      <c r="C58" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="5"/>
+      <c r="L58" s="2"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="4"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="5"/>
+      <c r="L59" s="2"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="4">
+        <v>43981</v>
+      </c>
+      <c r="B60" s="3"/>
+      <c r="C60" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="5"/>
+      <c r="L60" s="2"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="4"/>
+      <c r="B61" s="3">
+        <v>238</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J61" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K61" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L61" s="2"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="10">
+        <v>43982</v>
+      </c>
+      <c r="B62" s="11"/>
+      <c r="C62" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
+      <c r="G62" s="12"/>
+      <c r="H62" s="12"/>
+      <c r="I62" s="12"/>
+      <c r="J62" s="12"/>
+      <c r="K62" s="13"/>
+      <c r="L62" s="2"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="10"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="12"/>
+      <c r="H63" s="12"/>
+      <c r="I63" s="12"/>
+      <c r="J63" s="12"/>
+      <c r="K63" s="13"/>
+      <c r="L63" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D17433-4AC8-4D38-9E96-6A0FCAF256A8}">
+  <dimension ref="A1:L61"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="13.05078125" customWidth="1"/>
+    <col min="2" max="2" width="13.05078125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="75.47265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5234375" customWidth="1"/>
+    <col min="6" max="6" width="14.05078125" customWidth="1"/>
+    <col min="7" max="7" width="11.15625" customWidth="1"/>
+    <col min="8" max="8" width="9" customWidth="1"/>
+    <col min="9" max="9" width="10.15625" customWidth="1"/>
+    <col min="11" max="11" width="9.1015625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="4">
+        <v>43983</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="8"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="4"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="4">
+        <v>43984</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="4"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="4">
+        <v>43985</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="4"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="4">
+        <v>43986</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="4">
+        <v>43987</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="4"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="4">
+        <v>43988</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="4"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="4">
+        <v>43989</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="4"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="4">
+        <v>43990</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="4"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="4">
+        <v>43991</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="4"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="4">
+        <v>43992</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="4"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="4">
+        <v>43993</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="4"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="4">
+        <v>43994</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="4"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="4">
+        <v>43995</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="4"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="4">
+        <v>43996</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="4"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="4">
+        <v>43997</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="4"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="4">
+        <v>43998</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="4"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="4">
+        <v>43999</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="4"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="4">
+        <v>44000</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="4"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="4">
+        <v>44001</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="4"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="4">
+        <v>44002</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="4"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="4">
+        <v>44003</v>
+      </c>
+      <c r="B42" s="3"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="4"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="4">
+        <v>44004</v>
+      </c>
+      <c r="B44" s="3"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="2"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="4"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="2"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="4">
+        <v>44005</v>
+      </c>
+      <c r="B46" s="3"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="4"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="2"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="4">
+        <v>44006</v>
+      </c>
+      <c r="B48" s="3"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="2"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="4"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="2"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="4">
+        <v>44007</v>
+      </c>
+      <c r="B50" s="3"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="2"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="4"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="2"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="4">
+        <v>44008</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="2"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="4"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="2"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="4">
+        <v>44009</v>
+      </c>
+      <c r="B54" s="3"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="2"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="4"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="2"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="4">
+        <v>44010</v>
+      </c>
+      <c r="B56" s="3"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -5546,7 +6911,7 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="4">
-        <v>43980</v>
+        <v>44011</v>
       </c>
       <c r="B58" s="3"/>
       <c r="C58" s="2"/>
@@ -5576,7 +6941,7 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="4">
-        <v>43981</v>
+        <v>44012</v>
       </c>
       <c r="B60" s="3"/>
       <c r="C60" s="2"/>
@@ -5604,36 +6969,6 @@
       <c r="K61" s="5"/>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="10">
-        <v>43982</v>
-      </c>
-      <c r="B62" s="11"/>
-      <c r="C62" s="12"/>
-      <c r="D62" s="12"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
-      <c r="G62" s="12"/>
-      <c r="H62" s="12"/>
-      <c r="I62" s="12"/>
-      <c r="J62" s="12"/>
-      <c r="K62" s="13"/>
-      <c r="L62" s="2"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="10"/>
-      <c r="B63" s="11"/>
-      <c r="C63" s="12"/>
-      <c r="D63" s="12"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="12"/>
-      <c r="G63" s="12"/>
-      <c r="H63" s="12"/>
-      <c r="I63" s="12"/>
-      <c r="J63" s="12"/>
-      <c r="K63" s="13"/>
-      <c r="L63" s="12"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
problem 442, 448 finding the duplicates or missing values of range [1, n] in an array. Negate right location's value and traverse.
</commit_message>
<xml_diff>
--- a/Leetcode Team 403 Habiter.xlsx
+++ b/Leetcode Team 403 Habiter.xlsx
@@ -1,35 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E170FC5C-2398-41EA-B8F7-74B033B8E3FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E18F60-8F04-42EF-8B96-B733E9BFE4EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="March" sheetId="5" r:id="rId1"/>
     <sheet name="April" sheetId="4" r:id="rId2"/>
     <sheet name="May" sheetId="3" r:id="rId3"/>
     <sheet name="June" sheetId="6" r:id="rId4"/>
+    <sheet name="August" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="150">
   <si>
     <t>https://leetcode.com/problems/generate-parentheses/</t>
   </si>
@@ -473,13 +468,19 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/flatten-a-multilevel-doubly-linked-list/</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Negate right indexed value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -490,6 +491,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -653,13 +660,13 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="62">
+  <dxfs count="78">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1133,6 +1140,262 @@
     <dxf>
       <border outline="0">
         <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="20" formatCode="dd\-mmm\-yy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
           <color indexed="64"/>
         </top>
       </border>
@@ -1662,78 +1925,98 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C3B79F8F-34A5-48E2-A520-98D48807E864}" name="Table134" displayName="Table134" ref="A1:K63" totalsRowShown="0" headerRowDxfId="61" headerRowBorderDxfId="60" tableBorderDxfId="59" totalsRowBorderDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C3B79F8F-34A5-48E2-A520-98D48807E864}" name="Table134" displayName="Table134" ref="A1:K63" totalsRowShown="0" headerRowDxfId="77" headerRowBorderDxfId="76" tableBorderDxfId="75" totalsRowBorderDxfId="74">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B3E2ABC1-DFE4-41CF-B266-4C6F87E06327}" name="Date" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{D852D979-067D-4DC2-A8D3-F58D99FF98BA}" name="Problem #" dataDxfId="56"/>
-    <tableColumn id="3" xr3:uid="{7025E5D3-672C-4FA4-9F3F-E1B647279073}" name="Problem URL" dataDxfId="55"/>
-    <tableColumn id="4" xr3:uid="{F81AD9F7-6969-4C1D-82AF-E46E2DBC2668}" name="Difficulty" dataDxfId="54"/>
-    <tableColumn id="5" xr3:uid="{4C6862D0-7D2B-4C62-BB99-B3A2CEC64A5E}" name="Solved" dataDxfId="53"/>
-    <tableColumn id="6" xr3:uid="{72FF14F9-0236-434D-B7BC-F119041A3858}" name="Top Interviews" dataDxfId="52"/>
-    <tableColumn id="7" xr3:uid="{5C9B7229-C348-4A10-B7A7-1210D9FE0C0E}" name="Most Liked" dataDxfId="51"/>
-    <tableColumn id="8" xr3:uid="{94F9A000-47E5-4228-B070-3B2C13EB1AD1}" name="Amazon" dataDxfId="50"/>
-    <tableColumn id="9" xr3:uid="{92B0E2A3-76A8-4549-AA5D-108B4D679B77}" name="Facebook" dataDxfId="49"/>
-    <tableColumn id="10" xr3:uid="{6671C8FE-33F8-4C38-A35D-F4FF9BADAEC6}" name="Google" dataDxfId="48"/>
-    <tableColumn id="11" xr3:uid="{A31E59BF-042F-4790-B8E4-E936BED59AA3}" name="LinkedIn" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{B3E2ABC1-DFE4-41CF-B266-4C6F87E06327}" name="Date" dataDxfId="73"/>
+    <tableColumn id="2" xr3:uid="{D852D979-067D-4DC2-A8D3-F58D99FF98BA}" name="Problem #" dataDxfId="72"/>
+    <tableColumn id="3" xr3:uid="{7025E5D3-672C-4FA4-9F3F-E1B647279073}" name="Problem URL" dataDxfId="71"/>
+    <tableColumn id="4" xr3:uid="{F81AD9F7-6969-4C1D-82AF-E46E2DBC2668}" name="Difficulty" dataDxfId="70"/>
+    <tableColumn id="5" xr3:uid="{4C6862D0-7D2B-4C62-BB99-B3A2CEC64A5E}" name="Solved" dataDxfId="69"/>
+    <tableColumn id="6" xr3:uid="{72FF14F9-0236-434D-B7BC-F119041A3858}" name="Top Interviews" dataDxfId="68"/>
+    <tableColumn id="7" xr3:uid="{5C9B7229-C348-4A10-B7A7-1210D9FE0C0E}" name="Most Liked" dataDxfId="67"/>
+    <tableColumn id="8" xr3:uid="{94F9A000-47E5-4228-B070-3B2C13EB1AD1}" name="Amazon" dataDxfId="66"/>
+    <tableColumn id="9" xr3:uid="{92B0E2A3-76A8-4549-AA5D-108B4D679B77}" name="Facebook" dataDxfId="65"/>
+    <tableColumn id="10" xr3:uid="{6671C8FE-33F8-4C38-A35D-F4FF9BADAEC6}" name="Google" dataDxfId="64"/>
+    <tableColumn id="11" xr3:uid="{A31E59BF-042F-4790-B8E4-E936BED59AA3}" name="LinkedIn" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0549819D-3D5F-48EB-A65F-025354882917}" name="Table13" displayName="Table13" ref="A1:K61" totalsRowShown="0" headerRowDxfId="46" headerRowBorderDxfId="45" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0549819D-3D5F-48EB-A65F-025354882917}" name="Table13" displayName="Table13" ref="A1:K61" totalsRowShown="0" headerRowDxfId="62" headerRowBorderDxfId="61" tableBorderDxfId="60" totalsRowBorderDxfId="59">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{5CDA05DB-5000-4C00-A633-66BF5622D6CD}" name="Date" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{7C6B0860-8335-48BD-B7C1-AFB62305E598}" name="Problem #" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{FC1AE57B-B991-45CD-9BA8-367D5D66DDFC}" name="Problem URL" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{7B9C4890-7028-4D2D-A735-93498BD634DD}" name="Difficulty" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{A1BFF24E-EC8F-4F1D-8F03-8F7B483DFB42}" name="Solved" dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{195096CE-0E6A-414C-BC23-FC23890423A9}" name="Top Interviews" dataDxfId="37"/>
-    <tableColumn id="7" xr3:uid="{F0378ED8-CEEC-4E8E-BC9E-913A13A9AFFE}" name="Most Liked" dataDxfId="36"/>
-    <tableColumn id="8" xr3:uid="{0F66337C-7A88-4842-A889-3BD5E7F7082C}" name="Amazon" dataDxfId="35"/>
-    <tableColumn id="9" xr3:uid="{DEEF1C30-00D2-4B87-8A0F-96FA04079885}" name="Facebook" dataDxfId="34"/>
-    <tableColumn id="10" xr3:uid="{35C548D7-8613-4025-A49A-A1997303F552}" name="Google" dataDxfId="33"/>
-    <tableColumn id="11" xr3:uid="{D67985E4-DC76-475C-84B3-CA05145CF3C9}" name="LinkedIn" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{5CDA05DB-5000-4C00-A633-66BF5622D6CD}" name="Date" dataDxfId="58"/>
+    <tableColumn id="2" xr3:uid="{7C6B0860-8335-48BD-B7C1-AFB62305E598}" name="Problem #" dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{FC1AE57B-B991-45CD-9BA8-367D5D66DDFC}" name="Problem URL" dataDxfId="56"/>
+    <tableColumn id="4" xr3:uid="{7B9C4890-7028-4D2D-A735-93498BD634DD}" name="Difficulty" dataDxfId="55"/>
+    <tableColumn id="5" xr3:uid="{A1BFF24E-EC8F-4F1D-8F03-8F7B483DFB42}" name="Solved" dataDxfId="54"/>
+    <tableColumn id="6" xr3:uid="{195096CE-0E6A-414C-BC23-FC23890423A9}" name="Top Interviews" dataDxfId="53"/>
+    <tableColumn id="7" xr3:uid="{F0378ED8-CEEC-4E8E-BC9E-913A13A9AFFE}" name="Most Liked" dataDxfId="52"/>
+    <tableColumn id="8" xr3:uid="{0F66337C-7A88-4842-A889-3BD5E7F7082C}" name="Amazon" dataDxfId="51"/>
+    <tableColumn id="9" xr3:uid="{DEEF1C30-00D2-4B87-8A0F-96FA04079885}" name="Facebook" dataDxfId="50"/>
+    <tableColumn id="10" xr3:uid="{35C548D7-8613-4025-A49A-A1997303F552}" name="Google" dataDxfId="49"/>
+    <tableColumn id="11" xr3:uid="{D67985E4-DC76-475C-84B3-CA05145CF3C9}" name="LinkedIn" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C260067-204D-4DE0-B389-AD9BBC01A91C}" name="Table1" displayName="Table1" ref="A1:L63" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C260067-204D-4DE0-B389-AD9BBC01A91C}" name="Table1" displayName="Table1" ref="A1:L63" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{D97FE563-CFD8-462C-88F2-C01E4152DEEE}" name="Date" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{E9527249-09A4-424A-BAFE-0E7BC30662E1}" name="Problem #" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{8B765E68-8B4E-4BEF-82B4-EDB9783F6BDF}" name="Problem URL" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{13CD7928-4DED-4779-9896-BC43545F4337}" name="Difficulty" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{67FF5C2A-E60A-4705-9629-45553ABAA771}" name="Done" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{6A1310F5-514C-485B-A587-B9D947B9417F}" name="Top Interviews" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{3AA3576B-9804-4F97-8DD8-FF07619D454D}" name="Most Liked" dataDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{CBC2131C-26DD-4DD7-839B-3C7A594951E8}" name="Amazon" dataDxfId="20"/>
-    <tableColumn id="9" xr3:uid="{72326397-50FB-49F3-B00C-AA3D2AA10575}" name="Facebook" dataDxfId="19"/>
-    <tableColumn id="10" xr3:uid="{E82C2ABA-0938-4BF9-9AF0-AA05E888A695}" name="Google" dataDxfId="18"/>
-    <tableColumn id="11" xr3:uid="{31431F6E-7C6F-4646-8FFD-04F9FD89885E}" name="LinkedIn" dataDxfId="17"/>
-    <tableColumn id="12" xr3:uid="{946FB028-E4E2-424E-93DA-304146C527C2}" name="Column1" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{D97FE563-CFD8-462C-88F2-C01E4152DEEE}" name="Date" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{E9527249-09A4-424A-BAFE-0E7BC30662E1}" name="Problem #" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{8B765E68-8B4E-4BEF-82B4-EDB9783F6BDF}" name="Problem URL" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{13CD7928-4DED-4779-9896-BC43545F4337}" name="Difficulty" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{67FF5C2A-E60A-4705-9629-45553ABAA771}" name="Done" dataDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{6A1310F5-514C-485B-A587-B9D947B9417F}" name="Top Interviews" dataDxfId="38"/>
+    <tableColumn id="7" xr3:uid="{3AA3576B-9804-4F97-8DD8-FF07619D454D}" name="Most Liked" dataDxfId="37"/>
+    <tableColumn id="8" xr3:uid="{CBC2131C-26DD-4DD7-839B-3C7A594951E8}" name="Amazon" dataDxfId="36"/>
+    <tableColumn id="9" xr3:uid="{72326397-50FB-49F3-B00C-AA3D2AA10575}" name="Facebook" dataDxfId="35"/>
+    <tableColumn id="10" xr3:uid="{E82C2ABA-0938-4BF9-9AF0-AA05E888A695}" name="Google" dataDxfId="34"/>
+    <tableColumn id="11" xr3:uid="{31431F6E-7C6F-4646-8FFD-04F9FD89885E}" name="LinkedIn" dataDxfId="33"/>
+    <tableColumn id="12" xr3:uid="{946FB028-E4E2-424E-93DA-304146C527C2}" name="Note" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{34A5C7DE-E003-42F0-8FBE-3B98000334D8}" name="Table15" displayName="Table15" ref="A1:L61" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="13" tableBorderDxfId="14" totalsRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{34A5C7DE-E003-42F0-8FBE-3B98000334D8}" name="Table15" displayName="Table15" ref="A1:L61" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{A58CB880-41C7-4BDB-8A45-ACC4023CC087}" name="Date" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{C810554A-0AF3-4476-9084-1B8403573491}" name="Problem #" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{AE2548DB-F43F-4407-994C-C76E1C1015FE}" name="Problem URL" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{A55650E6-6475-48D6-9E1B-A53C50341856}" name="Difficulty" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{5BEC5DBF-C271-419C-8FF5-0BE151B16BC5}" name="Done" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{AEAE9C99-0023-4D64-8E36-4A81A1AAC3FB}" name="Top Interviews" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{41C684E6-D890-4F04-A167-9EB05CE52736}" name="Most Liked" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{D655B86E-CC8C-4581-A99E-946DC2107E3D}" name="Amazon" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{EDF1F749-934C-4AB3-B815-B4DB9E44725D}" name="Facebook" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{D4D114EB-F41E-418A-856F-EDC352E8854D}" name="Google" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{2666CAFC-3B33-4EBB-9A51-AD9CA119EDB5}" name="LinkedIn" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{7635171E-8EC8-436F-9264-9973B50380B5}" name="Column1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{A58CB880-41C7-4BDB-8A45-ACC4023CC087}" name="Date" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{C810554A-0AF3-4476-9084-1B8403573491}" name="Problem #" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{AE2548DB-F43F-4407-994C-C76E1C1015FE}" name="Problem URL" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{A55650E6-6475-48D6-9E1B-A53C50341856}" name="Difficulty" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{5BEC5DBF-C271-419C-8FF5-0BE151B16BC5}" name="Done" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{AEAE9C99-0023-4D64-8E36-4A81A1AAC3FB}" name="Top Interviews" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{41C684E6-D890-4F04-A167-9EB05CE52736}" name="Most Liked" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{D655B86E-CC8C-4581-A99E-946DC2107E3D}" name="Amazon" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{EDF1F749-934C-4AB3-B815-B4DB9E44725D}" name="Facebook" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{D4D114EB-F41E-418A-856F-EDC352E8854D}" name="Google" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{2666CAFC-3B33-4EBB-9A51-AD9CA119EDB5}" name="LinkedIn" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{7635171E-8EC8-436F-9264-9973B50380B5}" name="Column1" dataDxfId="16"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A26F2C86-6454-4073-ADD0-4CF9F3093E49}" name="Table156" displayName="Table156" ref="A1:L61" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="13" tableBorderDxfId="14" totalsRowBorderDxfId="12">
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{63764CA3-B68F-430A-B146-F3E9F3235F92}" name="Date" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{99585BF0-134D-4257-BFFF-EA373A588B36}" name="Problem #" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{110690FB-9E57-41CD-B331-4DCB8FB47A2F}" name="Problem URL" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{1783C987-1026-4E9D-A607-DF0B3D2CDC7C}" name="Difficulty" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{59275594-F606-4047-A96C-BB912350A8B1}" name="Done" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{B5D449FE-A69E-48A7-B376-EDDCD9A59469}" name="Top Interviews" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{B28BBD7A-DFDA-4641-B11D-3EB0029CAD58}" name="Most Liked" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{373F25D3-C54E-4DCD-BB46-5A5CDF34B240}" name="Amazon" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{4B29FB7F-3D9D-4D98-80C1-A1671871C58C}" name="Facebook" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{725408C3-99F9-45C0-B508-1AD590AAB0F0}" name="Google" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{38DD0071-6A10-4566-B0AE-1CB67E520C9F}" name="LinkedIn" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{940B1BD5-E1C4-46B0-8C14-62940848B718}" name="Note" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4423,11 +4706,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9570534-85A5-4387-8641-9D0197BC7F2B}">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C67" sqref="C67"/>
+      <selection pane="bottomRight" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4478,7 +4761,7 @@
         <v>94</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -5974,10 +6257,10 @@
   <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6342,6 +6625,1017 @@
         <v>43992</v>
       </c>
       <c r="B20" s="3"/>
+      <c r="C20" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="4"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="4">
+        <v>43993</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="4"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="4">
+        <v>43994</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="4"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="4">
+        <v>43995</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="4"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="4">
+        <v>43996</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="4"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="4">
+        <v>43997</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="4"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="4">
+        <v>43998</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="4"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="4">
+        <v>43999</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="4"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="4">
+        <v>44000</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="4"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="4">
+        <v>44001</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="4"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="4">
+        <v>44002</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="4"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="4">
+        <v>44003</v>
+      </c>
+      <c r="B42" s="3"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="4"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="4">
+        <v>44004</v>
+      </c>
+      <c r="B44" s="3"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="2"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="4"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="2"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="4">
+        <v>44005</v>
+      </c>
+      <c r="B46" s="3"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="4"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="2"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="4">
+        <v>44006</v>
+      </c>
+      <c r="B48" s="3"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="2"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="4"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="2"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="4">
+        <v>44007</v>
+      </c>
+      <c r="B50" s="3"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="2"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="4"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="2"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="4">
+        <v>44008</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="2"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="4"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="2"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="4">
+        <v>44009</v>
+      </c>
+      <c r="B54" s="3"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="2"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="4"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="2"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="4">
+        <v>44010</v>
+      </c>
+      <c r="B56" s="3"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="2"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="4"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="5"/>
+      <c r="L57" s="2"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="4">
+        <v>44011</v>
+      </c>
+      <c r="B58" s="3"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="5"/>
+      <c r="L58" s="2"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="4"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="5"/>
+      <c r="L59" s="2"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="4">
+        <v>44012</v>
+      </c>
+      <c r="B60" s="3"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="5"/>
+      <c r="L60" s="2"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="4"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="5"/>
+      <c r="L61" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3616B8FA-C35C-4892-9A7B-B66C7B927316}">
+  <dimension ref="A1:L61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="13.05078125" customWidth="1"/>
+    <col min="2" max="2" width="13.05078125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="75.47265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5234375" customWidth="1"/>
+    <col min="6" max="6" width="14.05078125" customWidth="1"/>
+    <col min="7" max="7" width="11.15625" customWidth="1"/>
+    <col min="8" max="8" width="9" customWidth="1"/>
+    <col min="9" max="9" width="10.15625" customWidth="1"/>
+    <col min="11" max="11" width="9.1015625" customWidth="1"/>
+    <col min="12" max="12" width="79.15625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="4">
+        <v>44044</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="8"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="4"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="4">
+        <v>44045</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="4"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="4">
+        <v>44046</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="4"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="4">
+        <v>44047</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="4">
+        <v>44048</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="4"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="4">
+        <v>44049</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="4"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="4">
+        <v>44050</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="4"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="4">
+        <v>44051</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="4"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="4">
+        <v>44052</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="4"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="4">
+        <v>44053</v>
+      </c>
+      <c r="B20" s="3"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -6369,7 +7663,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="4">
-        <v>43993</v>
+        <v>44054</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="20"/>
@@ -6399,7 +7693,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="4">
-        <v>43994</v>
+        <v>44055</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="2"/>
@@ -6429,7 +7723,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="4">
-        <v>43995</v>
+        <v>44056</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="2"/>
@@ -6459,10 +7753,10 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="4">
-        <v>43996</v>
+        <v>44057</v>
       </c>
       <c r="B28" s="3"/>
-      <c r="C28" s="2"/>
+      <c r="C28" s="14"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -6475,21 +7769,43 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="4"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="2"/>
+      <c r="B29" s="3">
+        <v>442</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="4">
-        <v>43997</v>
+        <v>44058</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="2"/>
@@ -6519,7 +7835,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="4">
-        <v>43998</v>
+        <v>44059</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="2"/>
@@ -6549,7 +7865,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="4">
-        <v>43999</v>
+        <v>44060</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="2"/>
@@ -6579,7 +7895,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="4">
-        <v>44000</v>
+        <v>44061</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="2"/>
@@ -6609,7 +7925,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="4">
-        <v>44001</v>
+        <v>44062</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="2"/>
@@ -6626,7 +7942,7 @@
     <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="4"/>
       <c r="B39" s="3"/>
-      <c r="C39" s="16"/>
+      <c r="C39" s="20"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
@@ -6639,7 +7955,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="4">
-        <v>44002</v>
+        <v>44063</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="2"/>
@@ -6656,7 +7972,7 @@
     <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="4"/>
       <c r="B41" s="3"/>
-      <c r="C41" s="16"/>
+      <c r="C41" s="20"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
@@ -6669,7 +7985,7 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="4">
-        <v>44003</v>
+        <v>44064</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="2"/>
@@ -6699,7 +8015,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="4">
-        <v>44004</v>
+        <v>44065</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="2"/>
@@ -6729,7 +8045,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="4">
-        <v>44005</v>
+        <v>44066</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="14"/>
@@ -6761,7 +8077,7 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="4">
-        <v>44006</v>
+        <v>44067</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="2"/>
@@ -6791,7 +8107,7 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="4">
-        <v>44007</v>
+        <v>44068</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="2"/>
@@ -6821,7 +8137,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="4">
-        <v>44008</v>
+        <v>44069</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="2"/>
@@ -6851,7 +8167,7 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="4">
-        <v>44009</v>
+        <v>44070</v>
       </c>
       <c r="B54" s="3"/>
       <c r="C54" s="2"/>
@@ -6881,7 +8197,7 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="4">
-        <v>44010</v>
+        <v>44071</v>
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="2"/>
@@ -6911,7 +8227,7 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="4">
-        <v>44011</v>
+        <v>44072</v>
       </c>
       <c r="B58" s="3"/>
       <c r="C58" s="2"/>
@@ -6941,7 +8257,7 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="4">
-        <v>44012</v>
+        <v>44073</v>
       </c>
       <c r="B60" s="3"/>
       <c r="C60" s="2"/>

</xml_diff>

<commit_message>
problem 449 Serialize deserialize BST. Preorder traversal with marker of leaf nodes.
</commit_message>
<xml_diff>
--- a/Leetcode Team 403 Habiter.xlsx
+++ b/Leetcode Team 403 Habiter.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E18F60-8F04-42EF-8B96-B733E9BFE4EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA99434A-2945-4645-BD4C-1C72D4D49C95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="151">
   <si>
     <t>https://leetcode.com/problems/generate-parentheses/</t>
   </si>
@@ -474,6 +474,9 @@
   </si>
   <si>
     <t>Negate right indexed value</t>
+  </si>
+  <si>
+    <t>Preorder traversal</t>
   </si>
 </sst>
 </file>
@@ -890,13 +893,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -906,6 +902,13 @@
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
@@ -2003,7 +2006,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A26F2C86-6454-4073-ADD0-4CF9F3093E49}" name="Table156" displayName="Table156" ref="A1:L61" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="13" tableBorderDxfId="14" totalsRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A26F2C86-6454-4073-ADD0-4CF9F3093E49}" name="Table156" displayName="Table156" ref="A1:L61" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12">
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{63764CA3-B68F-430A-B146-F3E9F3235F92}" name="Date" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{99585BF0-134D-4257-BFFF-EA373A588B36}" name="Problem #" dataDxfId="10"/>
@@ -7306,7 +7309,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomLeft" activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -7320,7 +7323,7 @@
     <col min="8" max="8" width="9" customWidth="1"/>
     <col min="9" max="9" width="10.15625" customWidth="1"/>
     <col min="11" max="11" width="9.1015625" customWidth="1"/>
-    <col min="12" max="12" width="79.15625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="37.20703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -7755,17 +7758,39 @@
       <c r="A28" s="4">
         <v>44057</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="2"/>
+      <c r="B28" s="3">
+        <v>449</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="4"/>

</xml_diff>

<commit_message>
problem 75 sort colors. Dutch Flag Partitioning Problem. Use three pointers r (first), w, b (last). Keep forwaring w and swapping with red or blue colors.
</commit_message>
<xml_diff>
--- a/Leetcode Team 403 Habiter.xlsx
+++ b/Leetcode Team 403 Habiter.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA99434A-2945-4645-BD4C-1C72D4D49C95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3FA7E2-AD5B-4FD7-BDC7-341932A2AB77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="152">
   <si>
     <t>https://leetcode.com/problems/generate-parentheses/</t>
   </si>
@@ -477,6 +477,9 @@
   </si>
   <si>
     <t>Preorder traversal</t>
+  </si>
+  <si>
+    <t>Dutch Flag Partitioning Problem; Two pointers</t>
   </si>
 </sst>
 </file>
@@ -7307,9 +7310,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3616B8FA-C35C-4892-9A7B-B66C7B927316}">
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L28" sqref="L28"/>
+      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -7742,17 +7745,39 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="4"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="2"/>
+      <c r="B27" s="3">
+        <v>75</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="4">

</xml_diff>

<commit_message>
problem 679 24 games. 4 numbers and 4 operators (parenthesis for picking a ordered pair of numbers) -> constant number of operations -> try backtracking
</commit_message>
<xml_diff>
--- a/Leetcode Team 403 Habiter.xlsx
+++ b/Leetcode Team 403 Habiter.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3FA7E2-AD5B-4FD7-BDC7-341932A2AB77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED206CF3-7715-4A67-84BD-E414263C7F42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="March" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="153">
   <si>
     <t>https://leetcode.com/problems/generate-parentheses/</t>
   </si>
@@ -480,6 +480,9 @@
   </si>
   <si>
     <t>Dutch Flag Partitioning Problem; Two pointers</t>
+  </si>
+  <si>
+    <t>Backtracking</t>
   </si>
 </sst>
 </file>
@@ -521,7 +524,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -640,12 +643,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -667,12 +683,269 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="78">
+  <dxfs count="79">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="20" formatCode="dd\-mmm\-yy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1679,244 +1952,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="20" formatCode="dd\-mmm\-yy"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1931,98 +1966,99 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C3B79F8F-34A5-48E2-A520-98D48807E864}" name="Table134" displayName="Table134" ref="A1:K63" totalsRowShown="0" headerRowDxfId="77" headerRowBorderDxfId="76" tableBorderDxfId="75" totalsRowBorderDxfId="74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C3B79F8F-34A5-48E2-A520-98D48807E864}" name="Table134" displayName="Table134" ref="A1:K63" totalsRowShown="0" headerRowDxfId="78" headerRowBorderDxfId="77" tableBorderDxfId="76" totalsRowBorderDxfId="75">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B3E2ABC1-DFE4-41CF-B266-4C6F87E06327}" name="Date" dataDxfId="73"/>
-    <tableColumn id="2" xr3:uid="{D852D979-067D-4DC2-A8D3-F58D99FF98BA}" name="Problem #" dataDxfId="72"/>
-    <tableColumn id="3" xr3:uid="{7025E5D3-672C-4FA4-9F3F-E1B647279073}" name="Problem URL" dataDxfId="71"/>
-    <tableColumn id="4" xr3:uid="{F81AD9F7-6969-4C1D-82AF-E46E2DBC2668}" name="Difficulty" dataDxfId="70"/>
-    <tableColumn id="5" xr3:uid="{4C6862D0-7D2B-4C62-BB99-B3A2CEC64A5E}" name="Solved" dataDxfId="69"/>
-    <tableColumn id="6" xr3:uid="{72FF14F9-0236-434D-B7BC-F119041A3858}" name="Top Interviews" dataDxfId="68"/>
-    <tableColumn id="7" xr3:uid="{5C9B7229-C348-4A10-B7A7-1210D9FE0C0E}" name="Most Liked" dataDxfId="67"/>
-    <tableColumn id="8" xr3:uid="{94F9A000-47E5-4228-B070-3B2C13EB1AD1}" name="Amazon" dataDxfId="66"/>
-    <tableColumn id="9" xr3:uid="{92B0E2A3-76A8-4549-AA5D-108B4D679B77}" name="Facebook" dataDxfId="65"/>
-    <tableColumn id="10" xr3:uid="{6671C8FE-33F8-4C38-A35D-F4FF9BADAEC6}" name="Google" dataDxfId="64"/>
-    <tableColumn id="11" xr3:uid="{A31E59BF-042F-4790-B8E4-E936BED59AA3}" name="LinkedIn" dataDxfId="63"/>
+    <tableColumn id="1" xr3:uid="{B3E2ABC1-DFE4-41CF-B266-4C6F87E06327}" name="Date" dataDxfId="74"/>
+    <tableColumn id="2" xr3:uid="{D852D979-067D-4DC2-A8D3-F58D99FF98BA}" name="Problem #" dataDxfId="73"/>
+    <tableColumn id="3" xr3:uid="{7025E5D3-672C-4FA4-9F3F-E1B647279073}" name="Problem URL" dataDxfId="72"/>
+    <tableColumn id="4" xr3:uid="{F81AD9F7-6969-4C1D-82AF-E46E2DBC2668}" name="Difficulty" dataDxfId="71"/>
+    <tableColumn id="5" xr3:uid="{4C6862D0-7D2B-4C62-BB99-B3A2CEC64A5E}" name="Solved" dataDxfId="70"/>
+    <tableColumn id="6" xr3:uid="{72FF14F9-0236-434D-B7BC-F119041A3858}" name="Top Interviews" dataDxfId="69"/>
+    <tableColumn id="7" xr3:uid="{5C9B7229-C348-4A10-B7A7-1210D9FE0C0E}" name="Most Liked" dataDxfId="68"/>
+    <tableColumn id="8" xr3:uid="{94F9A000-47E5-4228-B070-3B2C13EB1AD1}" name="Amazon" dataDxfId="67"/>
+    <tableColumn id="9" xr3:uid="{92B0E2A3-76A8-4549-AA5D-108B4D679B77}" name="Facebook" dataDxfId="66"/>
+    <tableColumn id="10" xr3:uid="{6671C8FE-33F8-4C38-A35D-F4FF9BADAEC6}" name="Google" dataDxfId="65"/>
+    <tableColumn id="11" xr3:uid="{A31E59BF-042F-4790-B8E4-E936BED59AA3}" name="LinkedIn" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0549819D-3D5F-48EB-A65F-025354882917}" name="Table13" displayName="Table13" ref="A1:K61" totalsRowShown="0" headerRowDxfId="62" headerRowBorderDxfId="61" tableBorderDxfId="60" totalsRowBorderDxfId="59">
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{5CDA05DB-5000-4C00-A633-66BF5622D6CD}" name="Date" dataDxfId="58"/>
-    <tableColumn id="2" xr3:uid="{7C6B0860-8335-48BD-B7C1-AFB62305E598}" name="Problem #" dataDxfId="57"/>
-    <tableColumn id="3" xr3:uid="{FC1AE57B-B991-45CD-9BA8-367D5D66DDFC}" name="Problem URL" dataDxfId="56"/>
-    <tableColumn id="4" xr3:uid="{7B9C4890-7028-4D2D-A735-93498BD634DD}" name="Difficulty" dataDxfId="55"/>
-    <tableColumn id="5" xr3:uid="{A1BFF24E-EC8F-4F1D-8F03-8F7B483DFB42}" name="Solved" dataDxfId="54"/>
-    <tableColumn id="6" xr3:uid="{195096CE-0E6A-414C-BC23-FC23890423A9}" name="Top Interviews" dataDxfId="53"/>
-    <tableColumn id="7" xr3:uid="{F0378ED8-CEEC-4E8E-BC9E-913A13A9AFFE}" name="Most Liked" dataDxfId="52"/>
-    <tableColumn id="8" xr3:uid="{0F66337C-7A88-4842-A889-3BD5E7F7082C}" name="Amazon" dataDxfId="51"/>
-    <tableColumn id="9" xr3:uid="{DEEF1C30-00D2-4B87-8A0F-96FA04079885}" name="Facebook" dataDxfId="50"/>
-    <tableColumn id="10" xr3:uid="{35C548D7-8613-4025-A49A-A1997303F552}" name="Google" dataDxfId="49"/>
-    <tableColumn id="11" xr3:uid="{D67985E4-DC76-475C-84B3-CA05145CF3C9}" name="LinkedIn" dataDxfId="48"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0549819D-3D5F-48EB-A65F-025354882917}" name="Table13" displayName="Table13" ref="A1:L61" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="13" tableBorderDxfId="14" totalsRowBorderDxfId="12">
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{5CDA05DB-5000-4C00-A633-66BF5622D6CD}" name="Date" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{7C6B0860-8335-48BD-B7C1-AFB62305E598}" name="Problem #" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{FC1AE57B-B991-45CD-9BA8-367D5D66DDFC}" name="Problem URL" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{7B9C4890-7028-4D2D-A735-93498BD634DD}" name="Difficulty" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{A1BFF24E-EC8F-4F1D-8F03-8F7B483DFB42}" name="Solved" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{195096CE-0E6A-414C-BC23-FC23890423A9}" name="Top Interviews" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{F0378ED8-CEEC-4E8E-BC9E-913A13A9AFFE}" name="Most Liked" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{0F66337C-7A88-4842-A889-3BD5E7F7082C}" name="Amazon" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{DEEF1C30-00D2-4B87-8A0F-96FA04079885}" name="Facebook" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{35C548D7-8613-4025-A49A-A1997303F552}" name="Google" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{D67985E4-DC76-475C-84B3-CA05145CF3C9}" name="LinkedIn" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{29BAC67F-A827-4CDC-8A52-7335CAF29E6C}" name="Column1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C260067-204D-4DE0-B389-AD9BBC01A91C}" name="Table1" displayName="Table1" ref="A1:L63" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C260067-204D-4DE0-B389-AD9BBC01A91C}" name="Table1" displayName="Table1" ref="A1:L63" totalsRowShown="0" headerRowDxfId="63" headerRowBorderDxfId="62" tableBorderDxfId="61" totalsRowBorderDxfId="60">
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{D97FE563-CFD8-462C-88F2-C01E4152DEEE}" name="Date" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{E9527249-09A4-424A-BAFE-0E7BC30662E1}" name="Problem #" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{8B765E68-8B4E-4BEF-82B4-EDB9783F6BDF}" name="Problem URL" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{13CD7928-4DED-4779-9896-BC43545F4337}" name="Difficulty" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{67FF5C2A-E60A-4705-9629-45553ABAA771}" name="Done" dataDxfId="39"/>
-    <tableColumn id="6" xr3:uid="{6A1310F5-514C-485B-A587-B9D947B9417F}" name="Top Interviews" dataDxfId="38"/>
-    <tableColumn id="7" xr3:uid="{3AA3576B-9804-4F97-8DD8-FF07619D454D}" name="Most Liked" dataDxfId="37"/>
-    <tableColumn id="8" xr3:uid="{CBC2131C-26DD-4DD7-839B-3C7A594951E8}" name="Amazon" dataDxfId="36"/>
-    <tableColumn id="9" xr3:uid="{72326397-50FB-49F3-B00C-AA3D2AA10575}" name="Facebook" dataDxfId="35"/>
-    <tableColumn id="10" xr3:uid="{E82C2ABA-0938-4BF9-9AF0-AA05E888A695}" name="Google" dataDxfId="34"/>
-    <tableColumn id="11" xr3:uid="{31431F6E-7C6F-4646-8FFD-04F9FD89885E}" name="LinkedIn" dataDxfId="33"/>
-    <tableColumn id="12" xr3:uid="{946FB028-E4E2-424E-93DA-304146C527C2}" name="Note" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{D97FE563-CFD8-462C-88F2-C01E4152DEEE}" name="Date" dataDxfId="59"/>
+    <tableColumn id="2" xr3:uid="{E9527249-09A4-424A-BAFE-0E7BC30662E1}" name="Problem #" dataDxfId="58"/>
+    <tableColumn id="3" xr3:uid="{8B765E68-8B4E-4BEF-82B4-EDB9783F6BDF}" name="Problem URL" dataDxfId="57"/>
+    <tableColumn id="4" xr3:uid="{13CD7928-4DED-4779-9896-BC43545F4337}" name="Difficulty" dataDxfId="56"/>
+    <tableColumn id="5" xr3:uid="{67FF5C2A-E60A-4705-9629-45553ABAA771}" name="Done" dataDxfId="55"/>
+    <tableColumn id="6" xr3:uid="{6A1310F5-514C-485B-A587-B9D947B9417F}" name="Top Interviews" dataDxfId="54"/>
+    <tableColumn id="7" xr3:uid="{3AA3576B-9804-4F97-8DD8-FF07619D454D}" name="Most Liked" dataDxfId="53"/>
+    <tableColumn id="8" xr3:uid="{CBC2131C-26DD-4DD7-839B-3C7A594951E8}" name="Amazon" dataDxfId="52"/>
+    <tableColumn id="9" xr3:uid="{72326397-50FB-49F3-B00C-AA3D2AA10575}" name="Facebook" dataDxfId="51"/>
+    <tableColumn id="10" xr3:uid="{E82C2ABA-0938-4BF9-9AF0-AA05E888A695}" name="Google" dataDxfId="50"/>
+    <tableColumn id="11" xr3:uid="{31431F6E-7C6F-4646-8FFD-04F9FD89885E}" name="LinkedIn" dataDxfId="49"/>
+    <tableColumn id="12" xr3:uid="{946FB028-E4E2-424E-93DA-304146C527C2}" name="Note" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{34A5C7DE-E003-42F0-8FBE-3B98000334D8}" name="Table15" displayName="Table15" ref="A1:L61" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{34A5C7DE-E003-42F0-8FBE-3B98000334D8}" name="Table15" displayName="Table15" ref="A1:L61" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{A58CB880-41C7-4BDB-8A45-ACC4023CC087}" name="Date" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{C810554A-0AF3-4476-9084-1B8403573491}" name="Problem #" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{AE2548DB-F43F-4407-994C-C76E1C1015FE}" name="Problem URL" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{A55650E6-6475-48D6-9E1B-A53C50341856}" name="Difficulty" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{5BEC5DBF-C271-419C-8FF5-0BE151B16BC5}" name="Done" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{AEAE9C99-0023-4D64-8E36-4A81A1AAC3FB}" name="Top Interviews" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{41C684E6-D890-4F04-A167-9EB05CE52736}" name="Most Liked" dataDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{D655B86E-CC8C-4581-A99E-946DC2107E3D}" name="Amazon" dataDxfId="20"/>
-    <tableColumn id="9" xr3:uid="{EDF1F749-934C-4AB3-B815-B4DB9E44725D}" name="Facebook" dataDxfId="19"/>
-    <tableColumn id="10" xr3:uid="{D4D114EB-F41E-418A-856F-EDC352E8854D}" name="Google" dataDxfId="18"/>
-    <tableColumn id="11" xr3:uid="{2666CAFC-3B33-4EBB-9A51-AD9CA119EDB5}" name="LinkedIn" dataDxfId="17"/>
-    <tableColumn id="12" xr3:uid="{7635171E-8EC8-436F-9264-9973B50380B5}" name="Column1" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{A58CB880-41C7-4BDB-8A45-ACC4023CC087}" name="Date" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{C810554A-0AF3-4476-9084-1B8403573491}" name="Problem #" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{AE2548DB-F43F-4407-994C-C76E1C1015FE}" name="Problem URL" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{A55650E6-6475-48D6-9E1B-A53C50341856}" name="Difficulty" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{5BEC5DBF-C271-419C-8FF5-0BE151B16BC5}" name="Done" dataDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{AEAE9C99-0023-4D64-8E36-4A81A1AAC3FB}" name="Top Interviews" dataDxfId="38"/>
+    <tableColumn id="7" xr3:uid="{41C684E6-D890-4F04-A167-9EB05CE52736}" name="Most Liked" dataDxfId="37"/>
+    <tableColumn id="8" xr3:uid="{D655B86E-CC8C-4581-A99E-946DC2107E3D}" name="Amazon" dataDxfId="36"/>
+    <tableColumn id="9" xr3:uid="{EDF1F749-934C-4AB3-B815-B4DB9E44725D}" name="Facebook" dataDxfId="35"/>
+    <tableColumn id="10" xr3:uid="{D4D114EB-F41E-418A-856F-EDC352E8854D}" name="Google" dataDxfId="34"/>
+    <tableColumn id="11" xr3:uid="{2666CAFC-3B33-4EBB-9A51-AD9CA119EDB5}" name="LinkedIn" dataDxfId="33"/>
+    <tableColumn id="12" xr3:uid="{7635171E-8EC8-436F-9264-9973B50380B5}" name="Column1" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A26F2C86-6454-4073-ADD0-4CF9F3093E49}" name="Table156" displayName="Table156" ref="A1:L61" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A26F2C86-6454-4073-ADD0-4CF9F3093E49}" name="Table156" displayName="Table156" ref="A1:L61" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{63764CA3-B68F-430A-B146-F3E9F3235F92}" name="Date" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{99585BF0-134D-4257-BFFF-EA373A588B36}" name="Problem #" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{110690FB-9E57-41CD-B331-4DCB8FB47A2F}" name="Problem URL" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{1783C987-1026-4E9D-A607-DF0B3D2CDC7C}" name="Difficulty" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{59275594-F606-4047-A96C-BB912350A8B1}" name="Done" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{B5D449FE-A69E-48A7-B376-EDDCD9A59469}" name="Top Interviews" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{B28BBD7A-DFDA-4641-B11D-3EB0029CAD58}" name="Most Liked" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{373F25D3-C54E-4DCD-BB46-5A5CDF34B240}" name="Amazon" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{4B29FB7F-3D9D-4D98-80C1-A1671871C58C}" name="Facebook" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{725408C3-99F9-45C0-B508-1AD590AAB0F0}" name="Google" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{38DD0071-6A10-4566-B0AE-1CB67E520C9F}" name="LinkedIn" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{940B1BD5-E1C4-46B0-8C14-62940848B718}" name="Note" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{63764CA3-B68F-430A-B146-F3E9F3235F92}" name="Date" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{99585BF0-134D-4257-BFFF-EA373A588B36}" name="Problem #" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{110690FB-9E57-41CD-B331-4DCB8FB47A2F}" name="Problem URL" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{1783C987-1026-4E9D-A607-DF0B3D2CDC7C}" name="Difficulty" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{59275594-F606-4047-A96C-BB912350A8B1}" name="Done" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{B5D449FE-A69E-48A7-B376-EDDCD9A59469}" name="Top Interviews" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{B28BBD7A-DFDA-4641-B11D-3EB0029CAD58}" name="Most Liked" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{373F25D3-C54E-4DCD-BB46-5A5CDF34B240}" name="Amazon" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{4B29FB7F-3D9D-4D98-80C1-A1671871C58C}" name="Facebook" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{725408C3-99F9-45C0-B508-1AD590AAB0F0}" name="Google" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{38DD0071-6A10-4566-B0AE-1CB67E520C9F}" name="LinkedIn" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{940B1BD5-E1C4-46B0-8C14-62940848B718}" name="Note" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2294,7 +2330,7 @@
   <dimension ref="A1:K65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B32" sqref="B32:K32"/>
@@ -3682,13 +3718,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA491B56-7F19-46F7-96DB-3602CC83D1F6}">
-  <dimension ref="A1:K61"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomRight" activeCell="K60" sqref="K60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3704,7 +3740,7 @@
     <col min="11" max="11" width="9.1015625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>82</v>
       </c>
@@ -3738,8 +3774,11 @@
       <c r="K1" s="9" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L1" s="21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4">
         <v>43922</v>
       </c>
@@ -3755,8 +3794,9 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="5"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L2" s="8"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4"/>
       <c r="B3" s="3"/>
       <c r="C3" s="2"/>
@@ -3768,8 +3808,9 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="5"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4">
         <v>43923</v>
       </c>
@@ -3785,8 +3826,9 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="5"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4"/>
       <c r="B5" s="3"/>
       <c r="C5" s="2" t="s">
@@ -3800,8 +3842,9 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="5"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4">
         <v>43924</v>
       </c>
@@ -3817,8 +3860,9 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="5"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4"/>
       <c r="B7" s="3"/>
       <c r="C7" s="2" t="s">
@@ -3832,8 +3876,9 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="5"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4">
         <v>43925</v>
       </c>
@@ -3849,8 +3894,9 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="5"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4"/>
       <c r="B9" s="3"/>
       <c r="C9" s="2" t="s">
@@ -3864,8 +3910,9 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="5"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4">
         <v>43926</v>
       </c>
@@ -3881,8 +3928,9 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="5"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4"/>
       <c r="B11" s="3"/>
       <c r="C11" s="2" t="s">
@@ -3896,8 +3944,9 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="5"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="4">
         <v>43927</v>
       </c>
@@ -3913,8 +3962,9 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="5"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="4"/>
       <c r="B13" s="3"/>
       <c r="C13" s="2" t="s">
@@ -3928,8 +3978,9 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="5"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="4">
         <v>43928</v>
       </c>
@@ -3945,8 +3996,9 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="4"/>
       <c r="B15" s="3"/>
       <c r="C15" s="2" t="s">
@@ -3960,8 +4012,9 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="5"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="4">
         <v>43929</v>
       </c>
@@ -3977,8 +4030,9 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="5"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="4"/>
       <c r="B17" s="3"/>
       <c r="C17" s="2" t="s">
@@ -3992,8 +4046,9 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="5"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="4">
         <v>43930</v>
       </c>
@@ -4009,8 +4064,9 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="5"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="4"/>
       <c r="B19" s="3"/>
       <c r="C19" s="2" t="s">
@@ -4024,8 +4080,9 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="5"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="4">
         <v>43931</v>
       </c>
@@ -4041,8 +4098,9 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="5"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="4"/>
       <c r="B21" s="3"/>
       <c r="C21" s="2" t="s">
@@ -4056,8 +4114,9 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="5"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="4">
         <v>43932</v>
       </c>
@@ -4073,8 +4132,9 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="5"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="4"/>
       <c r="B23" s="3"/>
       <c r="C23" s="2" t="s">
@@ -4088,8 +4148,9 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="5"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="4">
         <v>43933</v>
       </c>
@@ -4105,8 +4166,9 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="5"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="4"/>
       <c r="B25" s="3"/>
       <c r="C25" s="2" t="s">
@@ -4120,8 +4182,9 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="5"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="4">
         <v>43934</v>
       </c>
@@ -4137,8 +4200,9 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="5"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="4"/>
       <c r="B27" s="3"/>
       <c r="C27" s="2" t="s">
@@ -4152,8 +4216,9 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="5"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="4">
         <v>43935</v>
       </c>
@@ -4169,8 +4234,9 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="5"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="4"/>
       <c r="B29" s="3"/>
       <c r="C29" s="2" t="s">
@@ -4184,8 +4250,9 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="5"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="4">
         <v>43936</v>
       </c>
@@ -4201,8 +4268,9 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="5"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="4"/>
       <c r="B31" s="3"/>
       <c r="C31" s="2" t="s">
@@ -4216,8 +4284,9 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="5"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="4">
         <v>43937</v>
       </c>
@@ -4233,8 +4302,9 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="5"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="4"/>
       <c r="B33" s="3"/>
       <c r="C33" s="2" t="s">
@@ -4248,8 +4318,9 @@
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="5"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="4">
         <v>43938</v>
       </c>
@@ -4265,8 +4336,9 @@
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="5"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="4"/>
       <c r="B35" s="3"/>
       <c r="C35" s="2" t="s">
@@ -4280,8 +4352,9 @@
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="5"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="4">
         <v>43939</v>
       </c>
@@ -4297,8 +4370,9 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="5"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="2" t="s">
@@ -4312,8 +4386,9 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="5"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="4">
         <v>43940</v>
       </c>
@@ -4329,8 +4404,9 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="5"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="4"/>
       <c r="B39" s="3"/>
       <c r="C39" s="2" t="s">
@@ -4344,8 +4420,9 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="5"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="4">
         <v>43941</v>
       </c>
@@ -4361,8 +4438,9 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="5"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="4"/>
       <c r="B41" s="3"/>
       <c r="C41" s="2" t="s">
@@ -4376,8 +4454,9 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="5"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="4">
         <v>43942</v>
       </c>
@@ -4393,8 +4472,9 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="5"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="4"/>
       <c r="B43" s="3"/>
       <c r="C43" s="2" t="s">
@@ -4408,8 +4488,9 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="5"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="4">
         <v>43943</v>
       </c>
@@ -4425,8 +4506,9 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="5"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L44" s="2"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="4"/>
       <c r="B45" s="3"/>
       <c r="C45" s="2" t="s">
@@ -4440,8 +4522,9 @@
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="5"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L45" s="2"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="4">
         <v>43944</v>
       </c>
@@ -4457,8 +4540,9 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="5"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L46" s="2"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="4"/>
       <c r="B47" s="3"/>
       <c r="C47" s="2" t="s">
@@ -4472,8 +4556,9 @@
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="5"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L47" s="2"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="4">
         <v>43945</v>
       </c>
@@ -4489,8 +4574,9 @@
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="5"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L48" s="2"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="4"/>
       <c r="B49" s="3"/>
       <c r="C49" s="2" t="s">
@@ -4504,8 +4590,9 @@
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="5"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L49" s="2"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="4">
         <v>43946</v>
       </c>
@@ -4521,8 +4608,9 @@
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="5"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L50" s="2"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="4"/>
       <c r="B51" s="3"/>
       <c r="C51" s="2" t="s">
@@ -4536,8 +4624,9 @@
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="5"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L51" s="2"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="4">
         <v>43947</v>
       </c>
@@ -4553,8 +4642,9 @@
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
       <c r="K52" s="5"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L52" s="2"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="4"/>
       <c r="B53" s="3"/>
       <c r="C53" t="s">
@@ -4568,72 +4658,157 @@
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="5"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L53" s="2"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="4">
         <v>43948</v>
       </c>
-      <c r="B54" s="3"/>
+      <c r="B54" s="3">
+        <v>679</v>
+      </c>
       <c r="C54" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-      <c r="K54" s="5"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="D54" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="K54" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="4"/>
-      <c r="B55" s="3"/>
+      <c r="B55" s="3">
+        <v>75</v>
+      </c>
       <c r="C55" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
-      <c r="K55" s="5"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="D55" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K55" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L55" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="4">
         <v>43949</v>
       </c>
-      <c r="B56" s="3"/>
+      <c r="B56" s="3">
+        <v>449</v>
+      </c>
       <c r="C56" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
-      <c r="K56" s="5"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="D56" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K56" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L56" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="4"/>
-      <c r="B57" s="3"/>
+      <c r="B57" s="3">
+        <v>442</v>
+      </c>
       <c r="C57" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
-      <c r="H57" s="2"/>
-      <c r="I57" s="2"/>
-      <c r="J57" s="2"/>
-      <c r="K57" s="5"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="D57" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K57" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L57" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="4">
         <v>43950</v>
       </c>
@@ -4649,8 +4824,9 @@
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
       <c r="K58" s="5"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L58" s="2"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="4"/>
       <c r="B59" s="3"/>
       <c r="C59" s="2" t="s">
@@ -4664,8 +4840,9 @@
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
       <c r="K59" s="5"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L59" s="2"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="4">
         <v>43951</v>
       </c>
@@ -4681,8 +4858,9 @@
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
       <c r="K60" s="5"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L60" s="2"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="4"/>
       <c r="B61" s="3"/>
       <c r="C61" s="2" t="s">
@@ -4696,6 +4874,7 @@
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
       <c r="K61" s="5"/>
+      <c r="L61" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4713,7 +4892,7 @@
   <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="L1" sqref="L1"/>
@@ -6263,10 +6442,10 @@
   <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C39" sqref="C39"/>
+      <selection pane="bottomRight" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -7310,9 +7489,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3616B8FA-C35C-4892-9A7B-B66C7B927316}">
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -7731,17 +7910,39 @@
       <c r="A26" s="4">
         <v>44056</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="2"/>
+      <c r="B26" s="3">
+        <v>679</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="4"/>
@@ -8107,9 +8308,7 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="5"/>
-      <c r="L46" s="2" t="s">
-        <v>141</v>
-      </c>
+      <c r="L46" s="2"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="4"/>

</xml_diff>